<commit_message>
Fruit in progress - Haoyu 8/3
</commit_message>
<xml_diff>
--- a/Fruit/Data_sourse All tables/FruitYearbookGeneral_ATables.xlsx
+++ b/Fruit/Data_sourse All tables/FruitYearbookGeneral_ATables.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23001"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\SC\FRUIT\YRBOOK\Yrbook2019\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Haoyu Zhang\Desktop\Project2_Singh_Zhang_Zhang\Fruit\Data_sourse All tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E575CD3F-AB59-488C-9620-25369B20AB27}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11835" activeTab="7"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Content" sheetId="23" r:id="rId1"/>
@@ -106,17 +107,25 @@
     <definedName name="PRINT_AREA_MI">#REF!</definedName>
     <definedName name="tablea_1e">#REF!</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1715" uniqueCount="476">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1714" uniqueCount="475">
   <si>
     <t xml:space="preserve">  Crop</t>
   </si>
@@ -3501,9 +3510,6 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">                                               d</t>
-  </si>
-  <si>
     <t>* Total for all items will not match previous Yearbook issues due to the inclusion of melons. d = discontinued.</t>
   </si>
   <si>
@@ -3637,7 +3643,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="30">
     <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
@@ -4981,18 +4987,18 @@
   </cellXfs>
   <cellStyles count="13">
     <cellStyle name="Comma" xfId="12" builtinId="3"/>
-    <cellStyle name="Comma 2" xfId="2"/>
-    <cellStyle name="Comma 3" xfId="5"/>
+    <cellStyle name="Comma 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="Comma 3" xfId="5" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
     <cellStyle name="Hyperlink" xfId="10" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="3"/>
-    <cellStyle name="Normal 3" xfId="8"/>
-    <cellStyle name="Normal 4" xfId="9"/>
-    <cellStyle name="Normal 4 2" xfId="11"/>
-    <cellStyle name="Normal 5" xfId="6"/>
-    <cellStyle name="Normal 6" xfId="7"/>
-    <cellStyle name="Normal_A" xfId="4"/>
-    <cellStyle name="Normal_yrbooktaba-01" xfId="1"/>
+    <cellStyle name="Normal 2" xfId="3" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
+    <cellStyle name="Normal 3" xfId="8" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
+    <cellStyle name="Normal 4" xfId="9" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
+    <cellStyle name="Normal 4 2" xfId="11" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
+    <cellStyle name="Normal 5" xfId="6" xr:uid="{00000000-0005-0000-0000-000009000000}"/>
+    <cellStyle name="Normal 6" xfId="7" xr:uid="{00000000-0005-0000-0000-00000A000000}"/>
+    <cellStyle name="Normal_A" xfId="4" xr:uid="{00000000-0005-0000-0000-00000B000000}"/>
+    <cellStyle name="Normal_yrbooktaba-01" xfId="1" xr:uid="{00000000-0005-0000-0000-00000C000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -5269,7 +5275,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -5279,9 +5285,9 @@
       <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="110.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="110.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14">
@@ -5311,12 +5317,12 @@
     </row>
     <row r="6" spans="1:14">
       <c r="A6" s="375" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
     </row>
     <row r="7" spans="1:14">
       <c r="A7" s="371" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
     </row>
     <row r="8" spans="1:14">
@@ -5467,29 +5473,29 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A4" location="'taba-1b'!A1" display="Table A-1B--U.S. per capita use of selected, commercially produced, fresh, and processing fruit and tree nuts, 1976 to date "/>
-    <hyperlink ref="A5" location="'taba-1c'!A1" display="Table A-1C--U.S. per capita use of selected, commercially produced, fresh, and processing fruit and tree nuts, 1976 to date "/>
-    <hyperlink ref="A6" location="'taba-1d'!A1" display="Table A-1D--U.S. per capita use of selected, commercially produced, fresh, and processing fruit and tree nuts, 1976 to date "/>
-    <hyperlink ref="A8" location="'taba-2'!A1" display="Table A-2--Bearing acreage for fruit and tree nuts, United States, 1980 to date"/>
-    <hyperlink ref="A9" location="'taba-3'!A1" display="Table A-3--Utilized production and value of production of citrus and noncitrus fruit, United States, 1980 to date"/>
-    <hyperlink ref="A10" location="'taba-4'!A1" display="Table A-4--Bearing acreage for selected citrus and noncitrus fruit, United States, 1980 to date"/>
-    <hyperlink ref="A11" location="'taba-5'!A1" display="Table A-5--Total commercial production for selected citrus and noncitrus fruit, United States, 1980 to date"/>
-    <hyperlink ref="A12" location="'taba-6'!A1" display="Table A-6--Average price indexes, for fruit, Unites States, 1980 to date"/>
-    <hyperlink ref="A13" location="'taba-7'!A1" display="Table A-7--Annual average retail prices for selected fresh fruit, Unites States, 1980 to date"/>
-    <hyperlink ref="A14" location="'taba-8'!A1" display="Table A-8--Fruit and tree nuts: U.S. cash receipts, 1980 to date"/>
-    <hyperlink ref="A15" location="'taba-9'!A1" display="Table A-9--Fresh apples: U.S. monthly average retail price, marketing spread, and grower price, 1989 to date"/>
-    <hyperlink ref="A16" location="'taba-10'!A1" display="Table A-10--Fresh peaches: U.S. monthly average retail price, marketing spread, and grower price, 1989 to date"/>
-    <hyperlink ref="A17" location="'taba-11'!A1" display="Table A-11-- Fresh pears: U.S. monthly average retail price, marketing spread, and grower price, 1989 to date"/>
-    <hyperlink ref="A18" location="'taba-12'!A1" display="Table A-12--Fresh grapes: U.S. monthly average retail price, marketing spread, and grower price, 1995 to date"/>
-    <hyperlink ref="A19" location="'taba-13'!A1" display="Table A-13--Fresh strawberries: U.S. monthly average retail price, marketing spread, and grower price, 1989 to date"/>
-    <hyperlink ref="A20" location="'taba-14'!A1" display="Table A-14--Fresh oranges: U.S. monthly average retail price, marketing spread, and grower price, 1989/90 to date"/>
-    <hyperlink ref="A21" location="'taba-15'!A1" display="Table A-15--Fresh grapefruit: U.S. monthly average retail price, marketing spread, and grower price, 1989/90 to date"/>
-    <hyperlink ref="A22" location="'taba-16'!A1" display="Table A-16--Fresh lemons: U.S. monthly retail price, marketing spread, and grower price, 1989/90 to date"/>
-    <hyperlink ref="A23" location="'taba-17'!A1" display="Table A-17--Utilized production of selected fruit and tree nuts in the United States, by State, 2014"/>
-    <hyperlink ref="A24" location="'taba-18'!A1" display="Table A-18--Value of production for selected fruit and tree nuts in the United States, by State, 2014"/>
-    <hyperlink ref="A3" r:id="rId1" location="'taba-1a'!A1"/>
-    <hyperlink ref="A2" r:id="rId2" location="'taba-1a'!A1"/>
-    <hyperlink ref="A7" r:id="rId3"/>
+    <hyperlink ref="A4" location="'taba-1b'!A1" display="Table A-1B--U.S. per capita use of selected, commercially produced, fresh, and processing fruit and tree nuts, 1976 to date " xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="A5" location="'taba-1c'!A1" display="Table A-1C--U.S. per capita use of selected, commercially produced, fresh, and processing fruit and tree nuts, 1976 to date " xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="A6" location="'taba-1d'!A1" display="Table A-1D--U.S. per capita use of selected, commercially produced, fresh, and processing fruit and tree nuts, 1976 to date " xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="A8" location="'taba-2'!A1" display="Table A-2--Bearing acreage for fruit and tree nuts, United States, 1980 to date" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="A9" location="'taba-3'!A1" display="Table A-3--Utilized production and value of production of citrus and noncitrus fruit, United States, 1980 to date" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="A10" location="'taba-4'!A1" display="Table A-4--Bearing acreage for selected citrus and noncitrus fruit, United States, 1980 to date" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="A11" location="'taba-5'!A1" display="Table A-5--Total commercial production for selected citrus and noncitrus fruit, United States, 1980 to date" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="A12" location="'taba-6'!A1" display="Table A-6--Average price indexes, for fruit, Unites States, 1980 to date" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="A13" location="'taba-7'!A1" display="Table A-7--Annual average retail prices for selected fresh fruit, Unites States, 1980 to date" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="A14" location="'taba-8'!A1" display="Table A-8--Fruit and tree nuts: U.S. cash receipts, 1980 to date" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="A15" location="'taba-9'!A1" display="Table A-9--Fresh apples: U.S. monthly average retail price, marketing spread, and grower price, 1989 to date" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="A16" location="'taba-10'!A1" display="Table A-10--Fresh peaches: U.S. monthly average retail price, marketing spread, and grower price, 1989 to date" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="A17" location="'taba-11'!A1" display="Table A-11-- Fresh pears: U.S. monthly average retail price, marketing spread, and grower price, 1989 to date" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="A18" location="'taba-12'!A1" display="Table A-12--Fresh grapes: U.S. monthly average retail price, marketing spread, and grower price, 1995 to date" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="A19" location="'taba-13'!A1" display="Table A-13--Fresh strawberries: U.S. monthly average retail price, marketing spread, and grower price, 1989 to date" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="A20" location="'taba-14'!A1" display="Table A-14--Fresh oranges: U.S. monthly average retail price, marketing spread, and grower price, 1989/90 to date" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink ref="A21" location="'taba-15'!A1" display="Table A-15--Fresh grapefruit: U.S. monthly average retail price, marketing spread, and grower price, 1989/90 to date" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink ref="A22" location="'taba-16'!A1" display="Table A-16--Fresh lemons: U.S. monthly retail price, marketing spread, and grower price, 1989/90 to date" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
+    <hyperlink ref="A23" location="'taba-17'!A1" display="Table A-17--Utilized production of selected fruit and tree nuts in the United States, by State, 2014" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
+    <hyperlink ref="A24" location="'taba-18'!A1" display="Table A-18--Value of production for selected fruit and tree nuts in the United States, by State, 2014" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
+    <hyperlink ref="A3" r:id="rId1" location="'taba-1a'!A1" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
+    <hyperlink ref="A2" r:id="rId2" location="'taba-1a'!A1" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
+    <hyperlink ref="A7" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="83" orientation="portrait" r:id="rId4"/>
@@ -5497,7 +5503,7 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <sheetPr transitionEvaluation="1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -5507,14 +5513,14 @@
       <selection activeCell="O94" sqref="O94"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.7109375" defaultRowHeight="12"/>
+  <sheetFormatPr defaultColWidth="9.7265625" defaultRowHeight="11.5"/>
   <cols>
-    <col min="1" max="15" width="9.140625" style="160" customWidth="1"/>
-    <col min="16" max="16" width="12.85546875" style="160" customWidth="1"/>
-    <col min="17" max="17" width="14.7109375" style="160" customWidth="1"/>
-    <col min="18" max="18" width="10.7109375" style="160" customWidth="1"/>
-    <col min="19" max="19" width="13.140625" style="160" bestFit="1" customWidth="1"/>
-    <col min="20" max="16384" width="9.7109375" style="160"/>
+    <col min="1" max="15" width="9.1796875" style="160" customWidth="1"/>
+    <col min="16" max="16" width="12.81640625" style="160" customWidth="1"/>
+    <col min="17" max="17" width="14.7265625" style="160" customWidth="1"/>
+    <col min="18" max="18" width="10.7265625" style="160" customWidth="1"/>
+    <col min="19" max="19" width="13.1796875" style="160" bestFit="1" customWidth="1"/>
+    <col min="20" max="16384" width="9.7265625" style="160"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" s="111" customFormat="1" ht="10.15" customHeight="1">
@@ -5536,7 +5542,7 @@
       <c r="N1" s="109"/>
       <c r="O1" s="109"/>
     </row>
-    <row r="2" spans="1:17" s="111" customFormat="1" ht="3.95" customHeight="1">
+    <row r="2" spans="1:17" s="111" customFormat="1" ht="4" customHeight="1">
       <c r="A2" s="112"/>
       <c r="B2" s="113"/>
       <c r="C2" s="113"/>
@@ -5576,7 +5582,7 @@
       </c>
       <c r="N3" s="117"/>
     </row>
-    <row r="4" spans="1:17" s="111" customFormat="1" ht="12.95" customHeight="1">
+    <row r="4" spans="1:17" s="111" customFormat="1" ht="13" customHeight="1">
       <c r="A4" s="119" t="s">
         <v>107</v>
       </c>
@@ -5623,7 +5629,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="5" spans="1:17" s="111" customFormat="1" ht="3.95" customHeight="1">
+    <row r="5" spans="1:17" s="111" customFormat="1" ht="4" customHeight="1">
       <c r="A5" s="119"/>
       <c r="B5" s="118"/>
       <c r="C5" s="118"/>
@@ -6789,7 +6795,7 @@
       </c>
       <c r="Q30" s="168"/>
     </row>
-    <row r="31" spans="1:17" s="111" customFormat="1" ht="12.95" customHeight="1">
+    <row r="31" spans="1:17" s="111" customFormat="1" ht="13" customHeight="1">
       <c r="A31" s="112" t="s">
         <v>83</v>
       </c>
@@ -6838,7 +6844,7 @@
       </c>
       <c r="Q31" s="168"/>
     </row>
-    <row r="32" spans="1:17" s="111" customFormat="1" ht="12.95" customHeight="1">
+    <row r="32" spans="1:17" s="111" customFormat="1" ht="13" customHeight="1">
       <c r="A32" s="112" t="s">
         <v>84</v>
       </c>
@@ -6887,7 +6893,7 @@
       </c>
       <c r="Q32" s="168"/>
     </row>
-    <row r="33" spans="1:19" s="111" customFormat="1" ht="12.95" customHeight="1">
+    <row r="33" spans="1:19" s="111" customFormat="1" ht="13" customHeight="1">
       <c r="A33" s="112">
         <v>2005</v>
       </c>
@@ -6936,7 +6942,7 @@
       </c>
       <c r="Q33" s="168"/>
     </row>
-    <row r="34" spans="1:19" s="111" customFormat="1" ht="12.95" customHeight="1">
+    <row r="34" spans="1:19" s="111" customFormat="1" ht="13" customHeight="1">
       <c r="A34" s="112">
         <v>2006</v>
       </c>
@@ -6984,7 +6990,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="35" spans="1:19" s="111" customFormat="1" ht="12.95" customHeight="1">
+    <row r="35" spans="1:19" s="111" customFormat="1" ht="13" customHeight="1">
       <c r="A35" s="112">
         <v>2007</v>
       </c>
@@ -7033,7 +7039,7 @@
       </c>
       <c r="P35" s="169"/>
     </row>
-    <row r="36" spans="1:19" s="111" customFormat="1" ht="12.95" customHeight="1">
+    <row r="36" spans="1:19" s="111" customFormat="1" ht="13" customHeight="1">
       <c r="A36" s="112">
         <v>2008</v>
       </c>
@@ -7081,7 +7087,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="37" spans="1:19" s="111" customFormat="1" ht="12.95" customHeight="1">
+    <row r="37" spans="1:19" s="111" customFormat="1" ht="13" customHeight="1">
       <c r="A37" s="112">
         <v>2009</v>
       </c>
@@ -7129,7 +7135,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="38" spans="1:19" s="111" customFormat="1" ht="12.95" customHeight="1">
+    <row r="38" spans="1:19" s="111" customFormat="1" ht="13" customHeight="1">
       <c r="A38" s="112">
         <v>2010</v>
       </c>
@@ -7181,7 +7187,7 @@
       <c r="R38" s="497"/>
       <c r="S38" s="498"/>
     </row>
-    <row r="39" spans="1:19" s="111" customFormat="1" ht="12.95" customHeight="1">
+    <row r="39" spans="1:19" s="111" customFormat="1" ht="13" customHeight="1">
       <c r="A39" s="112">
         <v>2011</v>
       </c>
@@ -7232,7 +7238,7 @@
       <c r="Q39" s="498"/>
       <c r="R39" s="497"/>
     </row>
-    <row r="40" spans="1:19" s="111" customFormat="1" ht="12.95" customHeight="1">
+    <row r="40" spans="1:19" s="111" customFormat="1" ht="13" customHeight="1">
       <c r="A40" s="112" t="s">
         <v>85</v>
       </c>
@@ -7283,7 +7289,7 @@
       <c r="Q40" s="498"/>
       <c r="R40" s="497"/>
     </row>
-    <row r="41" spans="1:19" s="111" customFormat="1" ht="12.95" customHeight="1">
+    <row r="41" spans="1:19" s="111" customFormat="1" ht="13" customHeight="1">
       <c r="A41" s="112" t="s">
         <v>86</v>
       </c>
@@ -7334,7 +7340,7 @@
       <c r="Q41" s="498"/>
       <c r="R41" s="497"/>
     </row>
-    <row r="42" spans="1:19" s="111" customFormat="1" ht="12.95" customHeight="1">
+    <row r="42" spans="1:19" s="111" customFormat="1" ht="13" customHeight="1">
       <c r="A42" s="112">
         <v>2014</v>
       </c>
@@ -7385,7 +7391,7 @@
       <c r="Q42" s="498"/>
       <c r="R42" s="497"/>
     </row>
-    <row r="43" spans="1:19" s="111" customFormat="1" ht="12.95" customHeight="1">
+    <row r="43" spans="1:19" s="111" customFormat="1" ht="13" customHeight="1">
       <c r="A43" s="112">
         <v>2015</v>
       </c>
@@ -7436,7 +7442,7 @@
       <c r="Q43" s="498"/>
       <c r="R43" s="497"/>
     </row>
-    <row r="44" spans="1:19" s="111" customFormat="1" ht="12.95" customHeight="1">
+    <row r="44" spans="1:19" s="111" customFormat="1" ht="13" customHeight="1">
       <c r="A44" s="112">
         <v>2016</v>
       </c>
@@ -7487,7 +7493,7 @@
       <c r="Q44" s="498"/>
       <c r="R44" s="497"/>
     </row>
-    <row r="45" spans="1:19" s="111" customFormat="1" ht="12.95" customHeight="1">
+    <row r="45" spans="1:19" s="111" customFormat="1" ht="13" customHeight="1">
       <c r="A45" s="112">
         <v>2017</v>
       </c>
@@ -7538,7 +7544,7 @@
       <c r="Q45" s="498"/>
       <c r="R45" s="497"/>
     </row>
-    <row r="46" spans="1:19" s="111" customFormat="1" ht="12.95" customHeight="1">
+    <row r="46" spans="1:19" s="111" customFormat="1" ht="13" customHeight="1">
       <c r="A46" s="112">
         <v>2018</v>
       </c>
@@ -7633,7 +7639,7 @@
       <c r="N48" s="117"/>
       <c r="O48" s="117"/>
     </row>
-    <row r="49" spans="1:17" s="111" customFormat="1" ht="12.95" customHeight="1">
+    <row r="49" spans="1:17" s="111" customFormat="1" ht="13" customHeight="1">
       <c r="A49" s="119" t="s">
         <v>107</v>
       </c>
@@ -7680,7 +7686,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="50" spans="1:17" s="111" customFormat="1" ht="3.95" customHeight="1">
+    <row r="50" spans="1:17" s="111" customFormat="1" ht="4" customHeight="1">
       <c r="A50" s="119"/>
       <c r="B50" s="118"/>
       <c r="C50" s="118"/>
@@ -8233,7 +8239,7 @@
       </c>
       <c r="Q62" s="164"/>
     </row>
-    <row r="63" spans="1:17" s="111" customFormat="1" ht="12.95" customHeight="1">
+    <row r="63" spans="1:17" s="111" customFormat="1" ht="13" customHeight="1">
       <c r="A63" s="175">
         <v>1990</v>
       </c>
@@ -8284,7 +8290,7 @@
       </c>
       <c r="Q63" s="164"/>
     </row>
-    <row r="64" spans="1:17" s="111" customFormat="1" ht="12.95" customHeight="1">
+    <row r="64" spans="1:17" s="111" customFormat="1" ht="13" customHeight="1">
       <c r="A64" s="175">
         <v>1991</v>
       </c>
@@ -8333,7 +8339,7 @@
       </c>
       <c r="Q64" s="177"/>
     </row>
-    <row r="65" spans="1:30" s="111" customFormat="1" ht="12.95" customHeight="1">
+    <row r="65" spans="1:30" s="111" customFormat="1" ht="13" customHeight="1">
       <c r="A65" s="175">
         <v>1992</v>
       </c>
@@ -8382,7 +8388,7 @@
       </c>
       <c r="Q65" s="177"/>
     </row>
-    <row r="66" spans="1:30" s="111" customFormat="1" ht="12.95" customHeight="1">
+    <row r="66" spans="1:30" s="111" customFormat="1" ht="13" customHeight="1">
       <c r="A66" s="175">
         <v>1993</v>
       </c>
@@ -8431,7 +8437,7 @@
       </c>
       <c r="Q66" s="164"/>
     </row>
-    <row r="67" spans="1:30" s="111" customFormat="1" ht="12.95" customHeight="1">
+    <row r="67" spans="1:30" s="111" customFormat="1" ht="13" customHeight="1">
       <c r="A67" s="175">
         <v>1994</v>
       </c>
@@ -8480,7 +8486,7 @@
       </c>
       <c r="Q67" s="164"/>
     </row>
-    <row r="68" spans="1:30" s="111" customFormat="1" ht="12.95" customHeight="1">
+    <row r="68" spans="1:30" s="111" customFormat="1" ht="13" customHeight="1">
       <c r="A68" s="178">
         <v>1995</v>
       </c>
@@ -8530,7 +8536,7 @@
       </c>
       <c r="Q68" s="168"/>
     </row>
-    <row r="69" spans="1:30" s="111" customFormat="1" ht="12.95" customHeight="1">
+    <row r="69" spans="1:30" s="111" customFormat="1" ht="13" customHeight="1">
       <c r="A69" s="128">
         <v>1996</v>
       </c>
@@ -8580,7 +8586,7 @@
       </c>
       <c r="Q69" s="168"/>
     </row>
-    <row r="70" spans="1:30" s="111" customFormat="1" ht="12.95" customHeight="1">
+    <row r="70" spans="1:30" s="111" customFormat="1" ht="13" customHeight="1">
       <c r="A70" s="128">
         <v>1997</v>
       </c>
@@ -8633,7 +8639,7 @@
       <c r="S70" s="169"/>
       <c r="T70" s="169"/>
     </row>
-    <row r="71" spans="1:30" s="111" customFormat="1" ht="12.95" customHeight="1">
+    <row r="71" spans="1:30" s="111" customFormat="1" ht="13" customHeight="1">
       <c r="A71" s="128">
         <v>1998</v>
       </c>
@@ -8685,7 +8691,7 @@
       <c r="S71" s="169"/>
       <c r="T71" s="169"/>
     </row>
-    <row r="72" spans="1:30" s="111" customFormat="1" ht="12.95" customHeight="1">
+    <row r="72" spans="1:30" s="111" customFormat="1" ht="13" customHeight="1">
       <c r="A72" s="128">
         <v>1999</v>
       </c>
@@ -8737,7 +8743,7 @@
       <c r="S72" s="169"/>
       <c r="T72" s="169"/>
     </row>
-    <row r="73" spans="1:30" s="111" customFormat="1" ht="12.95" customHeight="1">
+    <row r="73" spans="1:30" s="111" customFormat="1" ht="13" customHeight="1">
       <c r="A73" s="178">
         <v>2000</v>
       </c>
@@ -8790,7 +8796,7 @@
       <c r="S73" s="169"/>
       <c r="T73" s="169"/>
     </row>
-    <row r="74" spans="1:30" s="111" customFormat="1" ht="12.95" customHeight="1">
+    <row r="74" spans="1:30" s="111" customFormat="1" ht="13" customHeight="1">
       <c r="A74" s="178">
         <v>2001</v>
       </c>
@@ -8843,7 +8849,7 @@
       <c r="S74" s="169"/>
       <c r="T74" s="169"/>
     </row>
-    <row r="75" spans="1:30" s="111" customFormat="1" ht="12.95" customHeight="1">
+    <row r="75" spans="1:30" s="111" customFormat="1" ht="13" customHeight="1">
       <c r="A75" s="178">
         <v>2002</v>
       </c>
@@ -8896,7 +8902,7 @@
       <c r="S75" s="169"/>
       <c r="T75" s="169"/>
     </row>
-    <row r="76" spans="1:30" s="111" customFormat="1" ht="12.95" customHeight="1">
+    <row r="76" spans="1:30" s="111" customFormat="1" ht="13" customHeight="1">
       <c r="A76" s="178">
         <v>2003</v>
       </c>
@@ -8949,7 +8955,7 @@
       <c r="S76" s="169"/>
       <c r="T76" s="169"/>
     </row>
-    <row r="77" spans="1:30" s="111" customFormat="1" ht="12.95" customHeight="1">
+    <row r="77" spans="1:30" s="111" customFormat="1" ht="13" customHeight="1">
       <c r="A77" s="178">
         <v>2004</v>
       </c>
@@ -9002,7 +9008,7 @@
       <c r="S77" s="169"/>
       <c r="T77" s="169"/>
     </row>
-    <row r="78" spans="1:30" s="111" customFormat="1" ht="12.95" customHeight="1">
+    <row r="78" spans="1:30" s="111" customFormat="1" ht="13" customHeight="1">
       <c r="A78" s="178">
         <v>2005</v>
       </c>
@@ -9055,7 +9061,7 @@
       <c r="S78" s="169"/>
       <c r="T78" s="169"/>
     </row>
-    <row r="79" spans="1:30" s="111" customFormat="1" ht="12.95" customHeight="1">
+    <row r="79" spans="1:30" s="111" customFormat="1" ht="13" customHeight="1">
       <c r="A79" s="178">
         <v>2006</v>
       </c>
@@ -9105,7 +9111,7 @@
       <c r="P79" s="180"/>
       <c r="Q79" s="168"/>
     </row>
-    <row r="80" spans="1:30" s="111" customFormat="1" ht="12.95" customHeight="1">
+    <row r="80" spans="1:30" s="111" customFormat="1" ht="13" customHeight="1">
       <c r="A80" s="178">
         <v>2007</v>
       </c>
@@ -9168,7 +9174,7 @@
       <c r="AC80" s="382"/>
       <c r="AD80" s="382"/>
     </row>
-    <row r="81" spans="1:30" s="111" customFormat="1" ht="12.95" customHeight="1">
+    <row r="81" spans="1:30" s="111" customFormat="1" ht="13" customHeight="1">
       <c r="A81" s="178">
         <v>2008</v>
       </c>
@@ -9231,7 +9237,7 @@
       <c r="AC81" s="382"/>
       <c r="AD81" s="382"/>
     </row>
-    <row r="82" spans="1:30" s="111" customFormat="1" ht="12.95" customHeight="1">
+    <row r="82" spans="1:30" s="111" customFormat="1" ht="13" customHeight="1">
       <c r="A82" s="178">
         <v>2009</v>
       </c>
@@ -9294,7 +9300,7 @@
       <c r="AC82" s="382"/>
       <c r="AD82" s="382"/>
     </row>
-    <row r="83" spans="1:30" s="111" customFormat="1" ht="12.95" customHeight="1">
+    <row r="83" spans="1:30" s="111" customFormat="1" ht="13" customHeight="1">
       <c r="A83" s="178">
         <v>2010</v>
       </c>
@@ -9357,7 +9363,7 @@
       <c r="AC83" s="382"/>
       <c r="AD83" s="382"/>
     </row>
-    <row r="84" spans="1:30" s="111" customFormat="1" ht="12.95" customHeight="1">
+    <row r="84" spans="1:30" s="111" customFormat="1" ht="13" customHeight="1">
       <c r="A84" s="181">
         <v>2011</v>
       </c>
@@ -9420,7 +9426,7 @@
       <c r="AC84" s="382"/>
       <c r="AD84" s="382"/>
     </row>
-    <row r="85" spans="1:30" s="111" customFormat="1" ht="12.95" customHeight="1">
+    <row r="85" spans="1:30" s="111" customFormat="1" ht="13" customHeight="1">
       <c r="A85" s="178">
         <v>2012</v>
       </c>
@@ -9482,7 +9488,7 @@
       <c r="AC85" s="382"/>
       <c r="AD85" s="382"/>
     </row>
-    <row r="86" spans="1:30" s="111" customFormat="1" ht="12.95" customHeight="1">
+    <row r="86" spans="1:30" s="111" customFormat="1" ht="13" customHeight="1">
       <c r="A86" s="178">
         <v>2013</v>
       </c>
@@ -9545,7 +9551,7 @@
       <c r="AC86" s="382"/>
       <c r="AD86" s="382"/>
     </row>
-    <row r="87" spans="1:30" s="111" customFormat="1" ht="12.95" customHeight="1">
+    <row r="87" spans="1:30" s="111" customFormat="1" ht="13" customHeight="1">
       <c r="A87" s="178">
         <v>2014</v>
       </c>
@@ -9608,7 +9614,7 @@
       <c r="AC87" s="382"/>
       <c r="AD87" s="382"/>
     </row>
-    <row r="88" spans="1:30" s="111" customFormat="1" ht="12.95" customHeight="1">
+    <row r="88" spans="1:30" s="111" customFormat="1" ht="13" customHeight="1">
       <c r="A88" s="178">
         <v>2015</v>
       </c>
@@ -9671,7 +9677,7 @@
       <c r="AC88" s="382"/>
       <c r="AD88" s="382"/>
     </row>
-    <row r="89" spans="1:30" s="111" customFormat="1" ht="12.95" customHeight="1">
+    <row r="89" spans="1:30" s="111" customFormat="1" ht="13" customHeight="1">
       <c r="A89" s="178">
         <v>2016</v>
       </c>
@@ -9734,7 +9740,7 @@
       <c r="AC89" s="382"/>
       <c r="AD89" s="382"/>
     </row>
-    <row r="90" spans="1:30" s="111" customFormat="1" ht="12.95" customHeight="1">
+    <row r="90" spans="1:30" s="111" customFormat="1" ht="13" customHeight="1">
       <c r="A90" s="178">
         <v>2017</v>
       </c>
@@ -9797,7 +9803,7 @@
       <c r="AC90" s="382"/>
       <c r="AD90" s="382"/>
     </row>
-    <row r="91" spans="1:30" s="111" customFormat="1" ht="12.95" customHeight="1">
+    <row r="91" spans="1:30" s="111" customFormat="1" ht="13" customHeight="1">
       <c r="A91" s="184">
         <v>2018</v>
       </c>
@@ -9860,7 +9866,7 @@
       <c r="AC91" s="382"/>
       <c r="AD91" s="382"/>
     </row>
-    <row r="92" spans="1:30" s="111" customFormat="1" ht="11.1" customHeight="1">
+    <row r="92" spans="1:30" s="111" customFormat="1" ht="11.15" customHeight="1">
       <c r="A92" s="191" t="s">
         <v>144</v>
       </c>
@@ -9881,7 +9887,7 @@
       <c r="Q92" s="168"/>
       <c r="R92" s="472"/>
     </row>
-    <row r="93" spans="1:30" s="111" customFormat="1" ht="12.95" customHeight="1">
+    <row r="93" spans="1:30" s="111" customFormat="1" ht="13" customHeight="1">
       <c r="A93" s="193" t="s">
         <v>425</v>
       </c>
@@ -9927,7 +9933,7 @@
       <c r="S94" s="169"/>
       <c r="T94" s="169"/>
     </row>
-    <row r="95" spans="1:30" ht="11.1" customHeight="1">
+    <row r="95" spans="1:30" ht="11.15" customHeight="1">
       <c r="A95" s="57" t="s">
         <v>146</v>
       </c>
@@ -9940,7 +9946,7 @@
       <c r="H95" s="194"/>
       <c r="I95" s="194"/>
     </row>
-    <row r="96" spans="1:30" ht="10.35" customHeight="1">
+    <row r="96" spans="1:30" ht="10.4" customHeight="1">
       <c r="A96" s="57"/>
       <c r="B96" s="194"/>
       <c r="C96" s="194"/>
@@ -9951,7 +9957,7 @@
       <c r="H96" s="194"/>
       <c r="I96" s="194"/>
     </row>
-    <row r="97" spans="1:10" ht="10.35" customHeight="1">
+    <row r="97" spans="1:10" ht="10.4" customHeight="1">
       <c r="A97" s="57"/>
       <c r="B97" s="194"/>
       <c r="C97" s="194"/>
@@ -9962,7 +9968,7 @@
       <c r="H97" s="194"/>
       <c r="I97" s="194"/>
     </row>
-    <row r="98" spans="1:10" ht="10.35" customHeight="1">
+    <row r="98" spans="1:10" ht="10.4" customHeight="1">
       <c r="A98" s="57"/>
       <c r="B98" s="194"/>
       <c r="C98" s="194"/>
@@ -10032,7 +10038,7 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <sheetPr transitionEvaluation="1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -10042,15 +10048,15 @@
       <selection activeCell="R38" sqref="R38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.7109375" defaultRowHeight="12"/>
+  <sheetFormatPr defaultColWidth="9.7265625" defaultRowHeight="11.5"/>
   <cols>
-    <col min="1" max="1" width="13.7109375" style="44" customWidth="1"/>
+    <col min="1" max="1" width="13.7265625" style="44" customWidth="1"/>
     <col min="2" max="3" width="17" style="44" customWidth="1"/>
-    <col min="4" max="6" width="10.5703125" style="44" customWidth="1"/>
-    <col min="7" max="7" width="2.7109375" style="44" customWidth="1"/>
-    <col min="8" max="9" width="10.5703125" style="44" customWidth="1"/>
-    <col min="10" max="10" width="13.140625" style="44" customWidth="1"/>
-    <col min="11" max="16384" width="9.7109375" style="44"/>
+    <col min="4" max="6" width="10.54296875" style="44" customWidth="1"/>
+    <col min="7" max="7" width="2.7265625" style="44" customWidth="1"/>
+    <col min="8" max="9" width="10.54296875" style="44" customWidth="1"/>
+    <col min="10" max="10" width="13.1796875" style="44" customWidth="1"/>
+    <col min="11" max="16384" width="9.7265625" style="44"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" s="106" customFormat="1" ht="10.15" customHeight="1">
@@ -10117,7 +10123,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="4" spans="1:10" s="106" customFormat="1" ht="12.95" customHeight="1">
+    <row r="4" spans="1:10" s="106" customFormat="1" ht="13" customHeight="1">
       <c r="A4" s="43"/>
       <c r="B4" s="77" t="s">
         <v>162</v>
@@ -10145,7 +10151,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="5" spans="1:10" s="106" customFormat="1" ht="3.95" customHeight="1">
+    <row r="5" spans="1:10" s="106" customFormat="1" ht="4" customHeight="1">
       <c r="A5" s="46"/>
       <c r="B5" s="52"/>
       <c r="C5" s="52"/>
@@ -11505,7 +11511,7 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <sheetPr transitionEvaluation="1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -11513,15 +11519,15 @@
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="11.5"/>
   <cols>
     <col min="1" max="1" width="7" style="44" customWidth="1"/>
-    <col min="2" max="2" width="11.5703125" style="44" customWidth="1"/>
-    <col min="3" max="3" width="10.7109375" style="44" customWidth="1"/>
-    <col min="4" max="4" width="11.5703125" style="44" customWidth="1"/>
-    <col min="5" max="5" width="13.42578125" style="44" customWidth="1"/>
-    <col min="6" max="9" width="11.5703125" style="44" customWidth="1"/>
-    <col min="10" max="16384" width="9.140625" style="44"/>
+    <col min="2" max="2" width="11.54296875" style="44" customWidth="1"/>
+    <col min="3" max="3" width="10.7265625" style="44" customWidth="1"/>
+    <col min="4" max="4" width="11.54296875" style="44" customWidth="1"/>
+    <col min="5" max="5" width="13.453125" style="44" customWidth="1"/>
+    <col min="6" max="9" width="11.54296875" style="44" customWidth="1"/>
+    <col min="10" max="16384" width="9.1796875" style="44"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="10.15" customHeight="1">
@@ -11537,7 +11543,7 @@
       <c r="H1" s="71"/>
       <c r="I1" s="71"/>
     </row>
-    <row r="2" spans="1:9" ht="3.95" customHeight="1">
+    <row r="2" spans="1:9" ht="4" customHeight="1">
       <c r="A2" s="51"/>
       <c r="B2" s="46"/>
       <c r="C2" s="46"/>
@@ -11596,7 +11602,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="3.95" customHeight="1">
+    <row r="5" spans="1:9" ht="4" customHeight="1">
       <c r="A5" s="48"/>
       <c r="B5" s="49"/>
       <c r="C5" s="48"/>
@@ -11607,7 +11613,7 @@
       <c r="H5" s="49"/>
       <c r="I5" s="49"/>
     </row>
-    <row r="6" spans="1:9" ht="3.95" customHeight="1">
+    <row r="6" spans="1:9" ht="4" customHeight="1">
       <c r="A6" s="51"/>
       <c r="B6" s="52"/>
       <c r="C6" s="51"/>
@@ -12873,7 +12879,7 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -12883,23 +12889,23 @@
       <selection activeCell="N48" sqref="N48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="11.5"/>
   <cols>
-    <col min="1" max="1" width="7.28515625" style="106" customWidth="1"/>
-    <col min="2" max="2" width="8.42578125" style="106" customWidth="1"/>
-    <col min="3" max="3" width="7.7109375" style="106" customWidth="1"/>
-    <col min="4" max="4" width="9.7109375" style="106" customWidth="1"/>
-    <col min="5" max="6" width="8.85546875" style="106" customWidth="1"/>
-    <col min="7" max="7" width="8.42578125" style="106" customWidth="1"/>
-    <col min="8" max="8" width="9.42578125" style="106" customWidth="1"/>
-    <col min="9" max="9" width="9.28515625" style="106" customWidth="1"/>
-    <col min="10" max="10" width="8.5703125" style="106" customWidth="1"/>
-    <col min="11" max="11" width="9.42578125" style="106" customWidth="1"/>
+    <col min="1" max="1" width="7.26953125" style="106" customWidth="1"/>
+    <col min="2" max="2" width="8.453125" style="106" customWidth="1"/>
+    <col min="3" max="3" width="7.7265625" style="106" customWidth="1"/>
+    <col min="4" max="4" width="9.7265625" style="106" customWidth="1"/>
+    <col min="5" max="6" width="8.81640625" style="106" customWidth="1"/>
+    <col min="7" max="7" width="8.453125" style="106" customWidth="1"/>
+    <col min="8" max="8" width="9.453125" style="106" customWidth="1"/>
+    <col min="9" max="9" width="9.26953125" style="106" customWidth="1"/>
+    <col min="10" max="10" width="8.54296875" style="106" customWidth="1"/>
+    <col min="11" max="11" width="9.453125" style="106" customWidth="1"/>
     <col min="12" max="12" width="10" style="106" customWidth="1"/>
-    <col min="13" max="14" width="9.85546875" style="106" customWidth="1"/>
+    <col min="13" max="14" width="9.81640625" style="106" customWidth="1"/>
     <col min="15" max="16" width="11" style="106" customWidth="1"/>
     <col min="17" max="18" width="11" style="106" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="13.5703125" style="106" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="13.54296875" style="106" bestFit="1" customWidth="1"/>
     <col min="20" max="16384" width="9" style="106"/>
   </cols>
   <sheetData>
@@ -12909,7 +12915,7 @@
       </c>
       <c r="N1" s="235"/>
     </row>
-    <row r="2" spans="1:14" ht="3.95" customHeight="1">
+    <row r="2" spans="1:14" ht="4" customHeight="1">
       <c r="A2" s="236"/>
       <c r="B2" s="237"/>
       <c r="C2" s="237"/>
@@ -12964,7 +12970,7 @@
       <c r="M3" s="243"/>
       <c r="N3" s="235"/>
     </row>
-    <row r="4" spans="1:14" ht="3.95" customHeight="1">
+    <row r="4" spans="1:14" ht="4" customHeight="1">
       <c r="A4" s="244"/>
       <c r="B4" s="243"/>
       <c r="C4" s="245"/>
@@ -12998,7 +13004,7 @@
       <c r="M5" s="243"/>
       <c r="N5" s="235"/>
     </row>
-    <row r="6" spans="1:14" ht="3.95" customHeight="1">
+    <row r="6" spans="1:14" ht="4" customHeight="1">
       <c r="A6" s="244"/>
       <c r="B6" s="243"/>
       <c r="C6" s="243"/>
@@ -13528,7 +13534,7 @@
       <c r="N20" s="235"/>
       <c r="O20" s="107"/>
     </row>
-    <row r="21" spans="1:15" ht="11.1" customHeight="1">
+    <row r="21" spans="1:15" ht="11.15" customHeight="1">
       <c r="A21" s="251" t="s">
         <v>57</v>
       </c>
@@ -13569,7 +13575,7 @@
       <c r="N21" s="235"/>
       <c r="O21" s="107"/>
     </row>
-    <row r="22" spans="1:15" ht="11.1" customHeight="1">
+    <row r="22" spans="1:15" ht="11.15" customHeight="1">
       <c r="A22" s="251" t="s">
         <v>58</v>
       </c>
@@ -13610,7 +13616,7 @@
       <c r="N22" s="235"/>
       <c r="O22" s="107"/>
     </row>
-    <row r="23" spans="1:15" ht="11.1" customHeight="1">
+    <row r="23" spans="1:15" ht="11.15" customHeight="1">
       <c r="A23" s="251" t="s">
         <v>59</v>
       </c>
@@ -13651,7 +13657,7 @@
       <c r="N23" s="235"/>
       <c r="O23" s="107"/>
     </row>
-    <row r="24" spans="1:15" ht="11.1" customHeight="1">
+    <row r="24" spans="1:15" ht="11.15" customHeight="1">
       <c r="A24" s="251" t="s">
         <v>122</v>
       </c>
@@ -13692,7 +13698,7 @@
       <c r="N24" s="235"/>
       <c r="O24" s="107"/>
     </row>
-    <row r="25" spans="1:15" ht="11.1" customHeight="1">
+    <row r="25" spans="1:15" ht="11.15" customHeight="1">
       <c r="A25" s="251" t="s">
         <v>61</v>
       </c>
@@ -13733,7 +13739,7 @@
       <c r="N25" s="235"/>
       <c r="O25" s="107"/>
     </row>
-    <row r="26" spans="1:15" ht="11.1" customHeight="1">
+    <row r="26" spans="1:15" ht="11.15" customHeight="1">
       <c r="A26" s="251" t="s">
         <v>62</v>
       </c>
@@ -13791,7 +13797,7 @@
       <c r="N27" s="235"/>
       <c r="O27" s="107"/>
     </row>
-    <row r="28" spans="1:15" ht="11.1" customHeight="1">
+    <row r="28" spans="1:15" ht="11.15" customHeight="1">
       <c r="A28" s="251" t="s">
         <v>63</v>
       </c>
@@ -13830,7 +13836,7 @@
       </c>
       <c r="M28" s="252"/>
     </row>
-    <row r="29" spans="1:15" ht="11.1" customHeight="1">
+    <row r="29" spans="1:15" ht="11.15" customHeight="1">
       <c r="A29" s="247" t="s">
         <v>64</v>
       </c>
@@ -13869,7 +13875,7 @@
       </c>
       <c r="M29" s="252"/>
     </row>
-    <row r="30" spans="1:15" ht="11.1" customHeight="1">
+    <row r="30" spans="1:15" ht="11.15" customHeight="1">
       <c r="A30" s="247" t="s">
         <v>65</v>
       </c>
@@ -13908,7 +13914,7 @@
       </c>
       <c r="M30" s="252"/>
     </row>
-    <row r="31" spans="1:15" ht="11.1" customHeight="1">
+    <row r="31" spans="1:15" ht="11.15" customHeight="1">
       <c r="A31" s="247" t="s">
         <v>66</v>
       </c>
@@ -13947,7 +13953,7 @@
       </c>
       <c r="M31" s="252"/>
     </row>
-    <row r="32" spans="1:15" ht="11.1" customHeight="1">
+    <row r="32" spans="1:15" ht="11.15" customHeight="1">
       <c r="A32" s="247" t="s">
         <v>67</v>
       </c>
@@ -13986,7 +13992,7 @@
       </c>
       <c r="M32" s="252"/>
     </row>
-    <row r="33" spans="1:19" ht="11.1" customHeight="1">
+    <row r="33" spans="1:19" ht="11.15" customHeight="1">
       <c r="A33" s="247" t="s">
         <v>83</v>
       </c>
@@ -14025,7 +14031,7 @@
       </c>
       <c r="M33" s="253"/>
     </row>
-    <row r="34" spans="1:19" ht="11.1" customHeight="1">
+    <row r="34" spans="1:19" ht="11.15" customHeight="1">
       <c r="A34" s="247" t="s">
         <v>84</v>
       </c>
@@ -14064,7 +14070,7 @@
       </c>
       <c r="M34" s="253"/>
     </row>
-    <row r="35" spans="1:19" ht="11.1" customHeight="1">
+    <row r="35" spans="1:19" ht="11.15" customHeight="1">
       <c r="A35" s="247" t="s">
         <v>192</v>
       </c>
@@ -14103,7 +14109,7 @@
       </c>
       <c r="M35" s="253"/>
     </row>
-    <row r="36" spans="1:19" ht="11.1" customHeight="1">
+    <row r="36" spans="1:19" ht="11.15" customHeight="1">
       <c r="A36" s="247" t="s">
         <v>193</v>
       </c>
@@ -14143,7 +14149,7 @@
       <c r="M36" s="253"/>
       <c r="S36" s="254"/>
     </row>
-    <row r="37" spans="1:19" ht="11.1" customHeight="1">
+    <row r="37" spans="1:19" ht="11.15" customHeight="1">
       <c r="A37" s="247" t="s">
         <v>194</v>
       </c>
@@ -14185,7 +14191,7 @@
       <c r="O37" s="107"/>
       <c r="S37" s="254"/>
     </row>
-    <row r="38" spans="1:19" ht="11.1" customHeight="1">
+    <row r="38" spans="1:19" ht="11.15" customHeight="1">
       <c r="A38" s="247" t="s">
         <v>195</v>
       </c>
@@ -14230,7 +14236,7 @@
       <c r="R38" s="256"/>
       <c r="S38" s="254"/>
     </row>
-    <row r="39" spans="1:19" ht="11.1" customHeight="1">
+    <row r="39" spans="1:19" ht="11.15" customHeight="1">
       <c r="A39" s="247" t="s">
         <v>196</v>
       </c>
@@ -14320,7 +14326,7 @@
       <c r="R40" s="256"/>
       <c r="S40" s="254"/>
     </row>
-    <row r="41" spans="1:19" ht="11.1" customHeight="1">
+    <row r="41" spans="1:19" ht="11.15" customHeight="1">
       <c r="A41" s="247" t="s">
         <v>198</v>
       </c>
@@ -14365,7 +14371,7 @@
       <c r="R41" s="256"/>
       <c r="S41" s="254"/>
     </row>
-    <row r="42" spans="1:19" ht="11.1" customHeight="1">
+    <row r="42" spans="1:19" ht="11.15" customHeight="1">
       <c r="A42" s="247" t="s">
         <v>199</v>
       </c>
@@ -14410,7 +14416,7 @@
       <c r="R42" s="256"/>
       <c r="S42" s="254"/>
     </row>
-    <row r="43" spans="1:19" ht="11.1" customHeight="1">
+    <row r="43" spans="1:19" ht="11.15" customHeight="1">
       <c r="A43" s="247" t="s">
         <v>200</v>
       </c>
@@ -14455,7 +14461,7 @@
       <c r="R43" s="256"/>
       <c r="S43" s="254"/>
     </row>
-    <row r="44" spans="1:19" ht="11.1" customHeight="1">
+    <row r="44" spans="1:19" ht="11.15" customHeight="1">
       <c r="A44" s="247" t="s">
         <v>201</v>
       </c>
@@ -14500,7 +14506,7 @@
       <c r="R44" s="256"/>
       <c r="S44" s="254"/>
     </row>
-    <row r="45" spans="1:19" ht="11.1" customHeight="1">
+    <row r="45" spans="1:19" ht="11.15" customHeight="1">
       <c r="A45" s="247" t="s">
         <v>418</v>
       </c>
@@ -14545,7 +14551,7 @@
       <c r="R45" s="256"/>
       <c r="S45" s="254"/>
     </row>
-    <row r="46" spans="1:19" ht="11.1" customHeight="1">
+    <row r="46" spans="1:19" ht="11.15" customHeight="1">
       <c r="A46" s="247" t="s">
         <v>427</v>
       </c>
@@ -14590,7 +14596,7 @@
       <c r="R46" s="256"/>
       <c r="S46" s="254"/>
     </row>
-    <row r="47" spans="1:19" ht="11.1" customHeight="1">
+    <row r="47" spans="1:19" ht="11.15" customHeight="1">
       <c r="A47" s="247" t="s">
         <v>451</v>
       </c>
@@ -14635,7 +14641,7 @@
       <c r="R47" s="256"/>
       <c r="S47" s="254"/>
     </row>
-    <row r="48" spans="1:19" ht="11.1" customHeight="1">
+    <row r="48" spans="1:19" ht="11.15" customHeight="1">
       <c r="A48" s="247" t="s">
         <v>463</v>
       </c>
@@ -14680,7 +14686,7 @@
       <c r="R48" s="256"/>
       <c r="S48" s="254"/>
     </row>
-    <row r="49" spans="1:19" ht="3.95" customHeight="1">
+    <row r="49" spans="1:19" ht="4" customHeight="1">
       <c r="A49" s="261"/>
       <c r="B49" s="253"/>
       <c r="C49" s="253"/>
@@ -14764,7 +14770,7 @@
       <c r="M51" s="243"/>
       <c r="N51" s="235"/>
     </row>
-    <row r="52" spans="1:19" ht="3.95" customHeight="1">
+    <row r="52" spans="1:19" ht="4" customHeight="1">
       <c r="A52" s="244"/>
       <c r="B52" s="246"/>
       <c r="C52" s="246"/>
@@ -14798,7 +14804,7 @@
       <c r="M53" s="243"/>
       <c r="N53" s="235"/>
     </row>
-    <row r="54" spans="1:19" ht="3.95" customHeight="1">
+    <row r="54" spans="1:19" ht="4" customHeight="1">
       <c r="A54" s="244"/>
       <c r="B54" s="243"/>
       <c r="C54" s="243"/>
@@ -15326,7 +15332,7 @@
       <c r="M68" s="250"/>
       <c r="N68" s="235"/>
     </row>
-    <row r="69" spans="1:18" ht="11.1" customHeight="1">
+    <row r="69" spans="1:18" ht="11.15" customHeight="1">
       <c r="A69" s="251" t="s">
         <v>57</v>
       </c>
@@ -15368,7 +15374,7 @@
       <c r="O69" s="107"/>
       <c r="P69" s="107"/>
     </row>
-    <row r="70" spans="1:18" ht="11.1" customHeight="1">
+    <row r="70" spans="1:18" ht="11.15" customHeight="1">
       <c r="A70" s="251" t="s">
         <v>58</v>
       </c>
@@ -15409,7 +15415,7 @@
       <c r="N70" s="235"/>
       <c r="O70" s="107"/>
     </row>
-    <row r="71" spans="1:18" ht="11.1" customHeight="1">
+    <row r="71" spans="1:18" ht="11.15" customHeight="1">
       <c r="A71" s="251" t="s">
         <v>59</v>
       </c>
@@ -15450,7 +15456,7 @@
       <c r="N71" s="235"/>
       <c r="O71" s="107"/>
     </row>
-    <row r="72" spans="1:18" s="266" customFormat="1" ht="11.1" customHeight="1">
+    <row r="72" spans="1:18" s="266" customFormat="1" ht="11.15" customHeight="1">
       <c r="A72" s="251" t="s">
         <v>122</v>
       </c>
@@ -15491,7 +15497,7 @@
       <c r="N72" s="265"/>
       <c r="O72" s="107"/>
     </row>
-    <row r="73" spans="1:18" s="266" customFormat="1" ht="11.1" customHeight="1">
+    <row r="73" spans="1:18" s="266" customFormat="1" ht="11.15" customHeight="1">
       <c r="A73" s="251" t="s">
         <v>61</v>
       </c>
@@ -15532,7 +15538,7 @@
       <c r="N73" s="265"/>
       <c r="O73" s="107"/>
     </row>
-    <row r="74" spans="1:18" s="266" customFormat="1" ht="11.1" customHeight="1">
+    <row r="74" spans="1:18" s="266" customFormat="1" ht="11.15" customHeight="1">
       <c r="A74" s="251" t="s">
         <v>62</v>
       </c>
@@ -15590,7 +15596,7 @@
       <c r="N75" s="265"/>
       <c r="O75" s="107"/>
     </row>
-    <row r="76" spans="1:18" ht="11.1" customHeight="1">
+    <row r="76" spans="1:18" ht="11.15" customHeight="1">
       <c r="A76" s="247" t="s">
         <v>63</v>
       </c>
@@ -15632,7 +15638,7 @@
       <c r="O76" s="107"/>
       <c r="P76" s="107"/>
     </row>
-    <row r="77" spans="1:18" ht="11.1" customHeight="1">
+    <row r="77" spans="1:18" ht="11.15" customHeight="1">
       <c r="A77" s="247" t="s">
         <v>64</v>
       </c>
@@ -15673,7 +15679,7 @@
       <c r="N77" s="235"/>
       <c r="O77" s="107"/>
     </row>
-    <row r="78" spans="1:18" ht="11.1" customHeight="1">
+    <row r="78" spans="1:18" ht="11.15" customHeight="1">
       <c r="A78" s="247" t="s">
         <v>65</v>
       </c>
@@ -15717,7 +15723,7 @@
       <c r="Q78" s="107"/>
       <c r="R78" s="107"/>
     </row>
-    <row r="79" spans="1:18" ht="11.1" customHeight="1">
+    <row r="79" spans="1:18" ht="11.15" customHeight="1">
       <c r="A79" s="247" t="s">
         <v>66</v>
       </c>
@@ -15761,7 +15767,7 @@
       <c r="Q79" s="107"/>
       <c r="R79" s="107"/>
     </row>
-    <row r="80" spans="1:18" ht="11.1" customHeight="1">
+    <row r="80" spans="1:18" ht="11.15" customHeight="1">
       <c r="A80" s="247" t="s">
         <v>67</v>
       </c>
@@ -15805,7 +15811,7 @@
       <c r="Q80" s="107"/>
       <c r="R80" s="107"/>
     </row>
-    <row r="81" spans="1:19" ht="11.1" customHeight="1">
+    <row r="81" spans="1:19" ht="11.15" customHeight="1">
       <c r="A81" s="247" t="s">
         <v>83</v>
       </c>
@@ -15849,7 +15855,7 @@
       <c r="Q81" s="107"/>
       <c r="R81" s="107"/>
     </row>
-    <row r="82" spans="1:19" ht="11.1" customHeight="1">
+    <row r="82" spans="1:19" ht="11.15" customHeight="1">
       <c r="A82" s="247" t="s">
         <v>84</v>
       </c>
@@ -15893,7 +15899,7 @@
       <c r="Q82" s="107"/>
       <c r="R82" s="107"/>
     </row>
-    <row r="83" spans="1:19" ht="11.1" customHeight="1">
+    <row r="83" spans="1:19" ht="11.15" customHeight="1">
       <c r="A83" s="247" t="s">
         <v>192</v>
       </c>
@@ -15937,7 +15943,7 @@
       <c r="Q83" s="107"/>
       <c r="R83" s="107"/>
     </row>
-    <row r="84" spans="1:19" ht="11.1" customHeight="1">
+    <row r="84" spans="1:19" ht="11.15" customHeight="1">
       <c r="A84" s="247" t="s">
         <v>193</v>
       </c>
@@ -15981,7 +15987,7 @@
       <c r="Q84" s="107"/>
       <c r="R84" s="107"/>
     </row>
-    <row r="85" spans="1:19" ht="11.1" customHeight="1">
+    <row r="85" spans="1:19" ht="11.15" customHeight="1">
       <c r="A85" s="247" t="s">
         <v>194</v>
       </c>
@@ -16025,7 +16031,7 @@
       <c r="Q85" s="107"/>
       <c r="R85" s="107"/>
     </row>
-    <row r="86" spans="1:19" ht="11.1" customHeight="1">
+    <row r="86" spans="1:19" ht="11.15" customHeight="1">
       <c r="A86" s="247" t="s">
         <v>195</v>
       </c>
@@ -16069,7 +16075,7 @@
       <c r="Q86" s="107"/>
       <c r="R86" s="107"/>
     </row>
-    <row r="87" spans="1:19" ht="11.1" customHeight="1">
+    <row r="87" spans="1:19" ht="11.15" customHeight="1">
       <c r="A87" s="247" t="s">
         <v>196</v>
       </c>
@@ -16113,7 +16119,7 @@
       <c r="Q87" s="107"/>
       <c r="R87" s="107"/>
     </row>
-    <row r="88" spans="1:19" ht="11.1" customHeight="1">
+    <row r="88" spans="1:19" ht="11.15" customHeight="1">
       <c r="A88" s="247" t="s">
         <v>197</v>
       </c>
@@ -16157,7 +16163,7 @@
       <c r="Q88" s="107"/>
       <c r="R88" s="107"/>
     </row>
-    <row r="89" spans="1:19" ht="11.1" customHeight="1">
+    <row r="89" spans="1:19" ht="11.15" customHeight="1">
       <c r="A89" s="247" t="s">
         <v>198</v>
       </c>
@@ -16201,7 +16207,7 @@
       <c r="Q89" s="107"/>
       <c r="R89" s="107"/>
     </row>
-    <row r="90" spans="1:19" ht="11.1" customHeight="1">
+    <row r="90" spans="1:19" ht="11.15" customHeight="1">
       <c r="A90" s="247" t="s">
         <v>199</v>
       </c>
@@ -16246,7 +16252,7 @@
       <c r="R90" s="107"/>
       <c r="S90" s="256"/>
     </row>
-    <row r="91" spans="1:19" ht="11.1" customHeight="1">
+    <row r="91" spans="1:19" ht="11.15" customHeight="1">
       <c r="A91" s="247" t="s">
         <v>200</v>
       </c>
@@ -16290,7 +16296,7 @@
       <c r="Q91" s="107"/>
       <c r="R91" s="107"/>
     </row>
-    <row r="92" spans="1:19" ht="11.1" customHeight="1">
+    <row r="92" spans="1:19" ht="11.15" customHeight="1">
       <c r="A92" s="247" t="s">
         <v>201</v>
       </c>
@@ -16334,7 +16340,7 @@
       <c r="Q92" s="107"/>
       <c r="R92" s="107"/>
     </row>
-    <row r="93" spans="1:19" ht="11.1" customHeight="1">
+    <row r="93" spans="1:19" ht="11.15" customHeight="1">
       <c r="A93" s="247" t="s">
         <v>418</v>
       </c>
@@ -16378,7 +16384,7 @@
       <c r="Q93" s="107"/>
       <c r="R93" s="107"/>
     </row>
-    <row r="94" spans="1:19" ht="11.1" customHeight="1">
+    <row r="94" spans="1:19" ht="11.15" customHeight="1">
       <c r="A94" s="247" t="s">
         <v>427</v>
       </c>
@@ -16422,7 +16428,7 @@
       <c r="Q94" s="107"/>
       <c r="R94" s="107"/>
     </row>
-    <row r="95" spans="1:19" ht="11.1" customHeight="1">
+    <row r="95" spans="1:19" ht="11.15" customHeight="1">
       <c r="A95" s="247" t="s">
         <v>451</v>
       </c>
@@ -16466,7 +16472,7 @@
       <c r="Q95" s="107"/>
       <c r="R95" s="107"/>
     </row>
-    <row r="96" spans="1:19" ht="11.1" customHeight="1">
+    <row r="96" spans="1:19" ht="11.15" customHeight="1">
       <c r="A96" s="242" t="s">
         <v>463</v>
       </c>
@@ -16510,7 +16516,7 @@
       <c r="Q96" s="107"/>
       <c r="R96" s="107"/>
     </row>
-    <row r="97" spans="1:15" ht="11.1" customHeight="1">
+    <row r="97" spans="1:15" ht="11.15" customHeight="1">
       <c r="A97" s="69" t="s">
         <v>400</v>
       </c>
@@ -16528,7 +16534,7 @@
       <c r="N97" s="235"/>
       <c r="O97" s="107"/>
     </row>
-    <row r="98" spans="1:15" ht="11.1" customHeight="1">
+    <row r="98" spans="1:15" ht="11.15" customHeight="1">
       <c r="A98" s="69" t="s">
         <v>453</v>
       </c>
@@ -16546,20 +16552,20 @@
       <c r="N98" s="235"/>
       <c r="O98" s="107"/>
     </row>
-    <row r="99" spans="1:15" ht="11.1" customHeight="1">
+    <row r="99" spans="1:15" ht="11.15" customHeight="1">
       <c r="A99" s="69" t="s">
         <v>428</v>
       </c>
       <c r="N99" s="235"/>
     </row>
-    <row r="100" spans="1:15" ht="11.1" customHeight="1">
+    <row r="100" spans="1:15" ht="11.15" customHeight="1">
       <c r="A100" s="69" t="s">
         <v>429</v>
       </c>
       <c r="B100" s="53"/>
       <c r="N100" s="235"/>
     </row>
-    <row r="101" spans="1:15" ht="11.1" customHeight="1">
+    <row r="101" spans="1:15" ht="11.15" customHeight="1">
       <c r="A101" s="266" t="s">
         <v>214</v>
       </c>
@@ -16581,7 +16587,7 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -16591,19 +16597,19 @@
       <selection activeCell="P32" sqref="P32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="11.5"/>
   <cols>
-    <col min="1" max="2" width="16.140625" style="106" customWidth="1"/>
-    <col min="3" max="4" width="16.7109375" style="106" customWidth="1"/>
-    <col min="5" max="5" width="6.7109375" style="106" customWidth="1"/>
-    <col min="6" max="7" width="16.7109375" style="106" customWidth="1"/>
-    <col min="8" max="8" width="9.7109375" style="106" customWidth="1"/>
+    <col min="1" max="2" width="16.1796875" style="106" customWidth="1"/>
+    <col min="3" max="4" width="16.7265625" style="106" customWidth="1"/>
+    <col min="5" max="5" width="6.7265625" style="106" customWidth="1"/>
+    <col min="6" max="7" width="16.7265625" style="106" customWidth="1"/>
+    <col min="8" max="8" width="9.7265625" style="106" customWidth="1"/>
     <col min="9" max="11" width="9" style="106" customWidth="1"/>
-    <col min="12" max="12" width="2.42578125" style="106" customWidth="1"/>
+    <col min="12" max="12" width="2.453125" style="106" customWidth="1"/>
     <col min="13" max="16384" width="9" style="106"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17">
+    <row r="1" spans="1:17" ht="12.5">
       <c r="A1" s="65" t="s">
         <v>215</v>
       </c>
@@ -16651,7 +16657,7 @@
       <c r="H3" s="53"/>
       <c r="I3" s="53"/>
     </row>
-    <row r="4" spans="1:17">
+    <row r="4" spans="1:17" ht="12.5">
       <c r="A4" s="71" t="s">
         <v>107</v>
       </c>
@@ -16685,7 +16691,7 @@
       <c r="H5" s="53"/>
       <c r="I5" s="53"/>
     </row>
-    <row r="6" spans="1:17" s="201" customFormat="1">
+    <row r="6" spans="1:17" s="201" customFormat="1" ht="12">
       <c r="A6" s="80"/>
       <c r="B6" s="54" t="s">
         <v>223</v>
@@ -16714,7 +16720,7 @@
       <c r="H7" s="53"/>
       <c r="I7" s="53"/>
     </row>
-    <row r="8" spans="1:17" ht="11.45" customHeight="1">
+    <row r="8" spans="1:17" ht="11.5" customHeight="1">
       <c r="A8" s="53" t="s">
         <v>54</v>
       </c>
@@ -17287,7 +17293,7 @@
       <c r="I31" s="281"/>
       <c r="J31" s="282"/>
     </row>
-    <row r="32" spans="1:10">
+    <row r="32" spans="1:10" ht="12.5">
       <c r="A32" s="45">
         <v>2013</v>
       </c>
@@ -17407,7 +17413,7 @@
       <c r="I36" s="281"/>
       <c r="J36" s="282"/>
     </row>
-    <row r="37" spans="1:11">
+    <row r="37" spans="1:11" ht="12.5">
       <c r="A37" s="65">
         <v>2018</v>
       </c>
@@ -17572,7 +17578,7 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -17580,18 +17586,18 @@
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="11.5"/>
   <cols>
-    <col min="1" max="4" width="16.140625" style="106" customWidth="1"/>
-    <col min="5" max="5" width="7.7109375" style="106" customWidth="1"/>
-    <col min="6" max="7" width="16.140625" style="106" customWidth="1"/>
-    <col min="8" max="8" width="9.7109375" style="106" customWidth="1"/>
+    <col min="1" max="4" width="16.1796875" style="106" customWidth="1"/>
+    <col min="5" max="5" width="7.7265625" style="106" customWidth="1"/>
+    <col min="6" max="7" width="16.1796875" style="106" customWidth="1"/>
+    <col min="8" max="8" width="9.7265625" style="106" customWidth="1"/>
     <col min="9" max="9" width="12" style="106" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.42578125" style="106" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.453125" style="106" bestFit="1" customWidth="1"/>
     <col min="11" max="16384" width="9" style="106"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14">
+    <row r="1" spans="1:14" ht="12.5">
       <c r="A1" s="65" t="s">
         <v>231</v>
       </c>
@@ -17632,7 +17638,7 @@
       <c r="E3" s="53"/>
       <c r="F3" s="53"/>
     </row>
-    <row r="4" spans="1:14">
+    <row r="4" spans="1:14" ht="12.5">
       <c r="A4" s="71" t="s">
         <v>107</v>
       </c>
@@ -17662,7 +17668,7 @@
       <c r="F5" s="52"/>
       <c r="G5" s="52"/>
     </row>
-    <row r="6" spans="1:14" s="201" customFormat="1">
+    <row r="6" spans="1:14" s="201" customFormat="1" ht="12">
       <c r="A6" s="80"/>
       <c r="B6" s="54" t="s">
         <v>223</v>
@@ -17687,7 +17693,7 @@
       <c r="F7" s="47"/>
       <c r="G7" s="47"/>
     </row>
-    <row r="8" spans="1:14" ht="11.45" customHeight="1">
+    <row r="8" spans="1:14" ht="11.5" customHeight="1">
       <c r="A8" s="53" t="s">
         <v>54</v>
       </c>
@@ -17709,7 +17715,7 @@
       </c>
       <c r="H8" s="282"/>
     </row>
-    <row r="9" spans="1:14" ht="11.45" customHeight="1">
+    <row r="9" spans="1:14" ht="11.5" customHeight="1">
       <c r="A9" s="53" t="s">
         <v>55</v>
       </c>
@@ -17731,7 +17737,7 @@
       </c>
       <c r="H9" s="282"/>
     </row>
-    <row r="10" spans="1:14" ht="11.45" customHeight="1">
+    <row r="10" spans="1:14" ht="11.5" customHeight="1">
       <c r="A10" s="53" t="s">
         <v>56</v>
       </c>
@@ -17753,7 +17759,7 @@
       </c>
       <c r="H10" s="282"/>
     </row>
-    <row r="11" spans="1:14" ht="11.45" customHeight="1">
+    <row r="11" spans="1:14" ht="11.5" customHeight="1">
       <c r="A11" s="53" t="s">
         <v>57</v>
       </c>
@@ -17775,7 +17781,7 @@
       </c>
       <c r="H11" s="282"/>
     </row>
-    <row r="12" spans="1:14" ht="11.45" customHeight="1">
+    <row r="12" spans="1:14" ht="11.5" customHeight="1">
       <c r="A12" s="53" t="s">
         <v>58</v>
       </c>
@@ -17797,7 +17803,7 @@
       </c>
       <c r="H12" s="282"/>
     </row>
-    <row r="13" spans="1:14" ht="11.45" customHeight="1">
+    <row r="13" spans="1:14" ht="11.5" customHeight="1">
       <c r="A13" s="53" t="s">
         <v>59</v>
       </c>
@@ -17819,7 +17825,7 @@
       </c>
       <c r="H13" s="282"/>
     </row>
-    <row r="14" spans="1:14" ht="11.45" customHeight="1">
+    <row r="14" spans="1:14" ht="11.5" customHeight="1">
       <c r="A14" s="53" t="s">
         <v>122</v>
       </c>
@@ -17841,7 +17847,7 @@
       </c>
       <c r="H14" s="282"/>
     </row>
-    <row r="15" spans="1:14" ht="11.45" customHeight="1">
+    <row r="15" spans="1:14" ht="11.5" customHeight="1">
       <c r="A15" s="53" t="s">
         <v>61</v>
       </c>
@@ -17863,7 +17869,7 @@
       </c>
       <c r="H15" s="282"/>
     </row>
-    <row r="16" spans="1:14" ht="11.45" customHeight="1">
+    <row r="16" spans="1:14" ht="11.5" customHeight="1">
       <c r="A16" s="53" t="s">
         <v>62</v>
       </c>
@@ -17885,7 +17891,7 @@
       </c>
       <c r="H16" s="282"/>
     </row>
-    <row r="17" spans="1:10" ht="11.45" customHeight="1">
+    <row r="17" spans="1:10" ht="11.5" customHeight="1">
       <c r="A17" s="53" t="s">
         <v>63</v>
       </c>
@@ -17907,7 +17913,7 @@
       </c>
       <c r="H17" s="282"/>
     </row>
-    <row r="18" spans="1:10" ht="11.45" customHeight="1">
+    <row r="18" spans="1:10" ht="11.5" customHeight="1">
       <c r="A18" s="46" t="s">
         <v>64</v>
       </c>
@@ -17929,7 +17935,7 @@
       </c>
       <c r="H18" s="282"/>
     </row>
-    <row r="19" spans="1:10" ht="11.45" customHeight="1">
+    <row r="19" spans="1:10" ht="11.5" customHeight="1">
       <c r="A19" s="45" t="s">
         <v>65</v>
       </c>
@@ -17951,7 +17957,7 @@
       </c>
       <c r="H19" s="282"/>
     </row>
-    <row r="20" spans="1:10" ht="11.45" customHeight="1">
+    <row r="20" spans="1:10" ht="11.5" customHeight="1">
       <c r="A20" s="45" t="s">
         <v>66</v>
       </c>
@@ -17973,7 +17979,7 @@
       </c>
       <c r="H20" s="282"/>
     </row>
-    <row r="21" spans="1:10" ht="11.45" customHeight="1">
+    <row r="21" spans="1:10" ht="11.5" customHeight="1">
       <c r="A21" s="45" t="s">
         <v>67</v>
       </c>
@@ -17995,7 +18001,7 @@
       </c>
       <c r="H21" s="282"/>
     </row>
-    <row r="22" spans="1:10" ht="11.45" customHeight="1">
+    <row r="22" spans="1:10" ht="11.5" customHeight="1">
       <c r="A22" s="45" t="s">
         <v>83</v>
       </c>
@@ -18017,7 +18023,7 @@
       </c>
       <c r="H22" s="282"/>
     </row>
-    <row r="23" spans="1:10" ht="11.45" customHeight="1">
+    <row r="23" spans="1:10" ht="11.5" customHeight="1">
       <c r="A23" s="45" t="s">
         <v>84</v>
       </c>
@@ -18039,7 +18045,7 @@
       </c>
       <c r="H23" s="282"/>
     </row>
-    <row r="24" spans="1:10" ht="11.45" customHeight="1">
+    <row r="24" spans="1:10" ht="11.5" customHeight="1">
       <c r="A24" s="45" t="s">
         <v>192</v>
       </c>
@@ -18063,7 +18069,7 @@
       <c r="I24" s="295"/>
       <c r="J24" s="290"/>
     </row>
-    <row r="25" spans="1:10" ht="11.45" customHeight="1">
+    <row r="25" spans="1:10" ht="11.5" customHeight="1">
       <c r="A25" s="45" t="s">
         <v>193</v>
       </c>
@@ -18087,7 +18093,7 @@
       <c r="I25" s="295"/>
       <c r="J25" s="290"/>
     </row>
-    <row r="26" spans="1:10" ht="11.45" customHeight="1">
+    <row r="26" spans="1:10" ht="11.5" customHeight="1">
       <c r="A26" s="45" t="s">
         <v>194</v>
       </c>
@@ -18111,7 +18117,7 @@
       <c r="I26" s="295"/>
       <c r="J26" s="290"/>
     </row>
-    <row r="27" spans="1:10" ht="11.45" customHeight="1">
+    <row r="27" spans="1:10" ht="11.5" customHeight="1">
       <c r="A27" s="45">
         <v>2008</v>
       </c>
@@ -18135,7 +18141,7 @@
       <c r="I27" s="295"/>
       <c r="J27" s="290"/>
     </row>
-    <row r="28" spans="1:10" ht="11.45" customHeight="1">
+    <row r="28" spans="1:10" ht="11.5" customHeight="1">
       <c r="A28" s="45">
         <v>2009</v>
       </c>
@@ -18159,7 +18165,7 @@
       <c r="I28" s="295"/>
       <c r="J28" s="290"/>
     </row>
-    <row r="29" spans="1:10" ht="11.45" customHeight="1">
+    <row r="29" spans="1:10" ht="11.5" customHeight="1">
       <c r="A29" s="45">
         <v>2010</v>
       </c>
@@ -18183,7 +18189,7 @@
       <c r="I29" s="295"/>
       <c r="J29" s="290"/>
     </row>
-    <row r="30" spans="1:10" ht="11.45" customHeight="1">
+    <row r="30" spans="1:10" ht="11.5" customHeight="1">
       <c r="A30" s="45">
         <v>2011</v>
       </c>
@@ -18207,7 +18213,7 @@
       <c r="I30" s="295"/>
       <c r="J30" s="290"/>
     </row>
-    <row r="31" spans="1:10" ht="11.45" customHeight="1">
+    <row r="31" spans="1:10" ht="11.5" customHeight="1">
       <c r="A31" s="45">
         <v>2012</v>
       </c>
@@ -18255,7 +18261,7 @@
       <c r="I32" s="295"/>
       <c r="J32" s="290"/>
     </row>
-    <row r="33" spans="1:10" ht="11.45" customHeight="1">
+    <row r="33" spans="1:10" ht="11.5" customHeight="1">
       <c r="A33" s="45">
         <v>2014</v>
       </c>
@@ -18279,7 +18285,7 @@
       <c r="I33" s="295"/>
       <c r="J33" s="290"/>
     </row>
-    <row r="34" spans="1:10" ht="11.45" customHeight="1">
+    <row r="34" spans="1:10" ht="11.5" customHeight="1">
       <c r="A34" s="45">
         <v>2015</v>
       </c>
@@ -18303,7 +18309,7 @@
       <c r="I34" s="295"/>
       <c r="J34" s="290"/>
     </row>
-    <row r="35" spans="1:10" ht="11.45" customHeight="1">
+    <row r="35" spans="1:10" ht="11.5" customHeight="1">
       <c r="A35" s="45">
         <v>2016</v>
       </c>
@@ -18327,7 +18333,7 @@
       <c r="I35" s="295"/>
       <c r="J35" s="290"/>
     </row>
-    <row r="36" spans="1:10" ht="11.45" customHeight="1">
+    <row r="36" spans="1:10" ht="11.5" customHeight="1">
       <c r="A36" s="45">
         <v>2017</v>
       </c>
@@ -18351,7 +18357,7 @@
       <c r="I36" s="295"/>
       <c r="J36" s="290"/>
     </row>
-    <row r="37" spans="1:10" ht="11.45" customHeight="1">
+    <row r="37" spans="1:10" ht="11.5" customHeight="1">
       <c r="A37" s="65">
         <v>2018</v>
       </c>
@@ -18498,7 +18504,7 @@
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -18506,20 +18512,20 @@
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="11.5"/>
   <cols>
-    <col min="1" max="1" width="17.140625" style="106" customWidth="1"/>
-    <col min="2" max="2" width="16.140625" style="106" customWidth="1"/>
-    <col min="3" max="4" width="16.7109375" style="106" customWidth="1"/>
-    <col min="5" max="5" width="7.7109375" style="106" customWidth="1"/>
-    <col min="6" max="7" width="16.7109375" style="106" customWidth="1"/>
+    <col min="1" max="1" width="17.1796875" style="106" customWidth="1"/>
+    <col min="2" max="2" width="16.1796875" style="106" customWidth="1"/>
+    <col min="3" max="4" width="16.7265625" style="106" customWidth="1"/>
+    <col min="5" max="5" width="7.7265625" style="106" customWidth="1"/>
+    <col min="6" max="7" width="16.7265625" style="106" customWidth="1"/>
     <col min="8" max="8" width="9" style="106"/>
-    <col min="9" max="9" width="9.140625" style="106" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.42578125" style="106" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.1796875" style="106" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.453125" style="106" bestFit="1" customWidth="1"/>
     <col min="11" max="16384" width="9" style="106"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" ht="12.5">
       <c r="A1" s="65" t="s">
         <v>235</v>
       </c>
@@ -18560,7 +18566,7 @@
       <c r="H3" s="53"/>
       <c r="I3" s="53"/>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" ht="12.5">
       <c r="A4" s="71" t="s">
         <v>107</v>
       </c>
@@ -18594,7 +18600,7 @@
       <c r="H5" s="53"/>
       <c r="I5" s="53"/>
     </row>
-    <row r="6" spans="1:10" s="201" customFormat="1">
+    <row r="6" spans="1:10" s="201" customFormat="1" ht="12">
       <c r="A6" s="80"/>
       <c r="B6" s="54" t="s">
         <v>223</v>
@@ -19468,7 +19474,7 @@
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -19478,12 +19484,12 @@
       <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="11.5"/>
   <cols>
-    <col min="1" max="4" width="16.140625" style="106" customWidth="1"/>
-    <col min="5" max="5" width="7.7109375" style="106" customWidth="1"/>
-    <col min="6" max="7" width="16.140625" style="106" customWidth="1"/>
-    <col min="8" max="8" width="9.7109375" style="106" customWidth="1"/>
+    <col min="1" max="4" width="16.1796875" style="106" customWidth="1"/>
+    <col min="5" max="5" width="7.7265625" style="106" customWidth="1"/>
+    <col min="6" max="7" width="16.1796875" style="106" customWidth="1"/>
+    <col min="8" max="8" width="9.7265625" style="106" customWidth="1"/>
     <col min="9" max="11" width="9" style="106" customWidth="1"/>
     <col min="12" max="12" width="1" style="106" customWidth="1"/>
     <col min="13" max="16384" width="9" style="106"/>
@@ -20305,7 +20311,7 @@
 </file>
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -20315,18 +20321,18 @@
       <selection activeCell="M23" sqref="M23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="11.5"/>
   <cols>
-    <col min="1" max="4" width="16.140625" style="106" customWidth="1"/>
-    <col min="5" max="5" width="7.7109375" style="106" customWidth="1"/>
-    <col min="6" max="7" width="16.140625" style="106" customWidth="1"/>
-    <col min="8" max="8" width="9.7109375" style="106" customWidth="1"/>
+    <col min="1" max="4" width="16.1796875" style="106" customWidth="1"/>
+    <col min="5" max="5" width="7.7265625" style="106" customWidth="1"/>
+    <col min="6" max="7" width="16.1796875" style="106" customWidth="1"/>
+    <col min="8" max="8" width="9.7265625" style="106" customWidth="1"/>
     <col min="9" max="11" width="9" style="106" customWidth="1"/>
-    <col min="12" max="12" width="0.85546875" style="106" customWidth="1"/>
+    <col min="12" max="12" width="0.81640625" style="106" customWidth="1"/>
     <col min="13" max="16384" width="9" style="106"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" ht="12.5">
       <c r="A1" s="65" t="s">
         <v>422</v>
       </c>
@@ -20363,7 +20369,7 @@
       <c r="E3" s="53"/>
       <c r="F3" s="53"/>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" ht="12.5">
       <c r="A4" s="71" t="s">
         <v>107</v>
       </c>
@@ -20393,7 +20399,7 @@
       <c r="F5" s="52"/>
       <c r="G5" s="52"/>
     </row>
-    <row r="6" spans="1:10" s="201" customFormat="1">
+    <row r="6" spans="1:10" s="201" customFormat="1" ht="12">
       <c r="A6" s="80"/>
       <c r="B6" s="54" t="s">
         <v>223</v>
@@ -21238,7 +21244,7 @@
 </file>
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -21248,16 +21254,16 @@
       <selection activeCell="M26" sqref="M26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="11.5"/>
   <cols>
-    <col min="1" max="2" width="16.140625" style="44" customWidth="1"/>
-    <col min="3" max="4" width="16.7109375" style="44" customWidth="1"/>
-    <col min="5" max="5" width="7.7109375" style="44" customWidth="1"/>
-    <col min="6" max="7" width="16.7109375" style="44" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" style="44"/>
+    <col min="1" max="2" width="16.1796875" style="44" customWidth="1"/>
+    <col min="3" max="4" width="16.7265625" style="44" customWidth="1"/>
+    <col min="5" max="5" width="7.7265625" style="44" customWidth="1"/>
+    <col min="6" max="7" width="16.7265625" style="44" customWidth="1"/>
+    <col min="8" max="16384" width="9.1796875" style="44"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16">
+    <row r="1" spans="1:16" ht="12.5">
       <c r="A1" s="65" t="s">
         <v>244</v>
       </c>
@@ -21314,7 +21320,7 @@
       <c r="J3" s="305"/>
       <c r="K3" s="305"/>
     </row>
-    <row r="4" spans="1:16">
+    <row r="4" spans="1:16" ht="12.5">
       <c r="A4" s="71" t="s">
         <v>245</v>
       </c>
@@ -21352,7 +21358,7 @@
       <c r="J5" s="305"/>
       <c r="K5" s="305"/>
     </row>
-    <row r="6" spans="1:16" s="84" customFormat="1">
+    <row r="6" spans="1:16" s="84" customFormat="1" ht="12">
       <c r="A6" s="80"/>
       <c r="B6" s="54" t="s">
         <v>223</v>
@@ -21811,7 +21817,7 @@
       <c r="J24" s="305"/>
       <c r="K24" s="305"/>
     </row>
-    <row r="25" spans="1:18" ht="12.75">
+    <row r="25" spans="1:18" ht="12.5">
       <c r="A25" s="45" t="s">
         <v>264</v>
       </c>
@@ -21842,7 +21848,7 @@
       <c r="Q25" s="308"/>
       <c r="R25" s="60"/>
     </row>
-    <row r="26" spans="1:18" ht="12.75">
+    <row r="26" spans="1:18" ht="12.5">
       <c r="A26" s="45" t="s">
         <v>265</v>
       </c>
@@ -22514,29 +22520,29 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr transitionEvaluation="1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:AL219"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="M42" sqref="M42"/>
+      <selection activeCell="K17" sqref="K17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="13.42578125" defaultRowHeight="9"/>
+  <sheetFormatPr defaultColWidth="13.453125" defaultRowHeight="9"/>
   <cols>
-    <col min="1" max="1" width="17.5703125" style="17" customWidth="1"/>
+    <col min="1" max="1" width="17.54296875" style="17" customWidth="1"/>
     <col min="2" max="11" width="8" style="17" customWidth="1"/>
     <col min="12" max="24" width="8" style="4" customWidth="1"/>
-    <col min="25" max="25" width="8.42578125" style="4" customWidth="1"/>
+    <col min="25" max="25" width="8.453125" style="4" customWidth="1"/>
     <col min="26" max="26" width="8" style="4" customWidth="1"/>
-    <col min="27" max="29" width="8.140625" style="4" customWidth="1"/>
-    <col min="30" max="38" width="13.42578125" style="4"/>
-    <col min="39" max="16384" width="13.42578125" style="17"/>
+    <col min="27" max="29" width="8.1796875" style="4" customWidth="1"/>
+    <col min="30" max="38" width="13.453125" style="4"/>
+    <col min="39" max="16384" width="13.453125" style="17"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" ht="10.35" customHeight="1">
+    <row r="1" spans="1:29" ht="10.4" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>466</v>
       </c>
@@ -22569,7 +22575,7 @@
       <c r="AB1" s="3"/>
       <c r="AC1" s="3"/>
     </row>
-    <row r="2" spans="1:29" ht="10.35" customHeight="1">
+    <row r="2" spans="1:29" ht="10.4" customHeight="1">
       <c r="A2" s="5" t="s">
         <v>0</v>
       </c>
@@ -22622,7 +22628,7 @@
       <c r="AB2" s="7"/>
       <c r="AC2" s="7"/>
     </row>
-    <row r="3" spans="1:29" ht="10.35" customHeight="1">
+    <row r="3" spans="1:29" ht="10.4" customHeight="1">
       <c r="A3" s="1"/>
       <c r="B3" s="8"/>
       <c r="C3" s="9"/>
@@ -26996,7 +27002,7 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -27006,18 +27012,18 @@
       <selection activeCell="L28" sqref="L28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="11.5"/>
   <cols>
-    <col min="1" max="4" width="16.140625" style="106" customWidth="1"/>
-    <col min="5" max="5" width="7.7109375" style="106" customWidth="1"/>
-    <col min="6" max="7" width="16.140625" style="106" customWidth="1"/>
-    <col min="8" max="8" width="9.7109375" style="106" customWidth="1"/>
+    <col min="1" max="4" width="16.1796875" style="106" customWidth="1"/>
+    <col min="5" max="5" width="7.7265625" style="106" customWidth="1"/>
+    <col min="6" max="7" width="16.1796875" style="106" customWidth="1"/>
+    <col min="8" max="8" width="9.7265625" style="106" customWidth="1"/>
     <col min="9" max="10" width="9" style="106" customWidth="1"/>
-    <col min="11" max="11" width="5.85546875" style="106" customWidth="1"/>
+    <col min="11" max="11" width="5.81640625" style="106" customWidth="1"/>
     <col min="12" max="16384" width="9" style="106"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15">
+    <row r="1" spans="1:15" ht="12.5">
       <c r="A1" s="65" t="s">
         <v>276</v>
       </c>
@@ -27065,7 +27071,7 @@
       <c r="I3" s="53"/>
       <c r="J3" s="53"/>
     </row>
-    <row r="4" spans="1:15">
+    <row r="4" spans="1:15" ht="12.5">
       <c r="A4" s="71" t="s">
         <v>245</v>
       </c>
@@ -27101,7 +27107,7 @@
       <c r="I5" s="53"/>
       <c r="J5" s="53"/>
     </row>
-    <row r="6" spans="1:15" s="201" customFormat="1">
+    <row r="6" spans="1:15" s="201" customFormat="1" ht="12">
       <c r="A6" s="80"/>
       <c r="B6" s="54" t="s">
         <v>223</v>
@@ -27953,7 +27959,7 @@
 </file>
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1400-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -27963,18 +27969,18 @@
       <selection activeCell="A42" sqref="A42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="11.5"/>
   <cols>
-    <col min="1" max="4" width="16.140625" style="106" customWidth="1"/>
-    <col min="5" max="5" width="7.7109375" style="106" customWidth="1"/>
-    <col min="6" max="7" width="16.140625" style="106" customWidth="1"/>
-    <col min="8" max="8" width="9.7109375" style="106" customWidth="1"/>
+    <col min="1" max="4" width="16.1796875" style="106" customWidth="1"/>
+    <col min="5" max="5" width="7.7265625" style="106" customWidth="1"/>
+    <col min="6" max="7" width="16.1796875" style="106" customWidth="1"/>
+    <col min="8" max="8" width="9.7265625" style="106" customWidth="1"/>
     <col min="9" max="10" width="9" style="106" customWidth="1"/>
-    <col min="11" max="11" width="5.85546875" style="106" customWidth="1"/>
+    <col min="11" max="11" width="5.81640625" style="106" customWidth="1"/>
     <col min="12" max="16384" width="9" style="106"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14">
+    <row r="1" spans="1:14" ht="12.5">
       <c r="A1" s="65" t="s">
         <v>287</v>
       </c>
@@ -28019,7 +28025,7 @@
       <c r="H3" s="53"/>
       <c r="I3" s="53"/>
     </row>
-    <row r="4" spans="1:14">
+    <row r="4" spans="1:14" ht="12.5">
       <c r="A4" s="71" t="s">
         <v>245</v>
       </c>
@@ -28053,7 +28059,7 @@
       <c r="H5" s="53"/>
       <c r="I5" s="53"/>
     </row>
-    <row r="6" spans="1:14" s="201" customFormat="1">
+    <row r="6" spans="1:14" s="201" customFormat="1" ht="12">
       <c r="A6" s="80"/>
       <c r="B6" s="54" t="s">
         <v>223</v>
@@ -28909,7 +28915,7 @@
 </file>
 
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1500-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -28922,16 +28928,16 @@
       <selection pane="bottomRight" activeCell="AH57" sqref="AH57"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="12.5"/>
   <cols>
-    <col min="1" max="1" width="12.7109375" style="397" customWidth="1"/>
-    <col min="2" max="37" width="10.7109375" style="397" customWidth="1"/>
-    <col min="38" max="38" width="11.7109375" style="397" customWidth="1"/>
-    <col min="39" max="39" width="9.140625" style="397"/>
-    <col min="40" max="40" width="11.28515625" style="397" bestFit="1" customWidth="1"/>
-    <col min="41" max="43" width="9.140625" style="397"/>
-    <col min="44" max="44" width="11.28515625" style="397" bestFit="1" customWidth="1"/>
-    <col min="45" max="16384" width="9.140625" style="397"/>
+    <col min="1" max="1" width="12.7265625" style="397" customWidth="1"/>
+    <col min="2" max="37" width="10.7265625" style="397" customWidth="1"/>
+    <col min="38" max="38" width="11.7265625" style="397" customWidth="1"/>
+    <col min="39" max="39" width="9.1796875" style="397"/>
+    <col min="40" max="40" width="11.26953125" style="397" bestFit="1" customWidth="1"/>
+    <col min="41" max="43" width="9.1796875" style="397"/>
+    <col min="44" max="44" width="11.26953125" style="397" bestFit="1" customWidth="1"/>
+    <col min="45" max="16384" width="9.1796875" style="397"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:44" ht="12.75" customHeight="1">
@@ -40368,7 +40374,7 @@
 </file>
 
 <file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1600-000000000000}">
   <dimension ref="A1:AY200"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
@@ -40378,21 +40384,21 @@
       <selection pane="bottomRight" activeCell="M17" sqref="M17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="12.5"/>
   <cols>
-    <col min="1" max="1" width="12.7109375" style="328" customWidth="1"/>
-    <col min="2" max="37" width="10.7109375" style="328" customWidth="1"/>
-    <col min="38" max="38" width="11.7109375" style="328" customWidth="1"/>
-    <col min="39" max="39" width="9.140625" style="328"/>
-    <col min="40" max="40" width="11.28515625" style="328" bestFit="1" customWidth="1"/>
-    <col min="41" max="43" width="9.140625" style="328"/>
-    <col min="44" max="44" width="11.28515625" style="328" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.7265625" style="328" customWidth="1"/>
+    <col min="2" max="37" width="10.7265625" style="328" customWidth="1"/>
+    <col min="38" max="38" width="11.7265625" style="328" customWidth="1"/>
+    <col min="39" max="39" width="9.1796875" style="328"/>
+    <col min="40" max="40" width="11.26953125" style="328" bestFit="1" customWidth="1"/>
+    <col min="41" max="43" width="9.1796875" style="328"/>
+    <col min="44" max="44" width="11.26953125" style="328" bestFit="1" customWidth="1"/>
     <col min="45" max="45" width="14" style="328" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="9.140625" style="328"/>
-    <col min="47" max="47" width="12.85546875" style="328" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="16.5703125" style="328" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="11.28515625" style="328" bestFit="1" customWidth="1"/>
-    <col min="50" max="16384" width="9.140625" style="328"/>
+    <col min="46" max="46" width="9.1796875" style="328"/>
+    <col min="47" max="47" width="12.81640625" style="328" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="16.54296875" style="328" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="11.26953125" style="328" bestFit="1" customWidth="1"/>
+    <col min="50" max="16384" width="9.1796875" style="328"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:51">
@@ -41179,7 +41185,7 @@
       <c r="AX9" s="357"/>
       <c r="AY9" s="357"/>
     </row>
-    <row r="10" spans="1:51" ht="15">
+    <row r="10" spans="1:51" ht="14.5">
       <c r="A10" s="339" t="s">
         <v>314</v>
       </c>
@@ -45152,7 +45158,7 @@
       <c r="AX40" s="357"/>
       <c r="AY40" s="357"/>
     </row>
-    <row r="41" spans="1:51" ht="15">
+    <row r="41" spans="1:51" ht="14.5">
       <c r="A41" s="339" t="s">
         <v>344</v>
       </c>
@@ -52287,20 +52293,20 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr transitionEvaluation="1"/>
   <dimension ref="A1:L93"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="120" zoomScaleNormal="120" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="13.42578125" defaultRowHeight="9"/>
+  <sheetFormatPr defaultColWidth="13.453125" defaultRowHeight="9"/>
   <cols>
-    <col min="1" max="1" width="17.5703125" style="17" customWidth="1"/>
-    <col min="2" max="11" width="9.140625" style="17" customWidth="1"/>
-    <col min="12" max="16384" width="13.42578125" style="17"/>
+    <col min="1" max="1" width="17.54296875" style="17" customWidth="1"/>
+    <col min="2" max="11" width="9.1796875" style="17" customWidth="1"/>
+    <col min="12" max="16384" width="13.453125" style="17"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="10.35" customHeight="1">
+    <row r="1" spans="1:12" ht="10.4" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>468</v>
       </c>
@@ -52314,7 +52320,7 @@
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
     </row>
-    <row r="2" spans="1:12" ht="10.35" customHeight="1">
+    <row r="2" spans="1:12" ht="10.4" customHeight="1">
       <c r="A2" s="5" t="s">
         <v>0</v>
       </c>
@@ -52349,7 +52355,7 @@
         <v>1995</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="10.35" customHeight="1">
+    <row r="3" spans="1:12" ht="10.4" customHeight="1">
       <c r="A3" s="1"/>
       <c r="B3" s="8"/>
       <c r="C3" s="10"/>
@@ -55064,20 +55070,20 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr transitionEvaluation="1"/>
   <dimension ref="A1:L98"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="120" zoomScaleNormal="120" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="13.42578125" defaultRowHeight="9"/>
+  <sheetFormatPr defaultColWidth="13.453125" defaultRowHeight="9"/>
   <cols>
-    <col min="1" max="1" width="17.5703125" style="17" customWidth="1"/>
-    <col min="2" max="11" width="9.140625" style="17" customWidth="1"/>
-    <col min="12" max="16384" width="13.42578125" style="17"/>
+    <col min="1" max="1" width="17.54296875" style="17" customWidth="1"/>
+    <col min="2" max="11" width="9.1796875" style="17" customWidth="1"/>
+    <col min="12" max="16384" width="13.453125" style="17"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="10.35" customHeight="1">
+    <row r="1" spans="1:12" ht="10.4" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>468</v>
       </c>
@@ -55090,7 +55096,7 @@
       <c r="H1" s="26"/>
       <c r="I1" s="26"/>
     </row>
-    <row r="2" spans="1:12" ht="10.35" customHeight="1">
+    <row r="2" spans="1:12" ht="10.4" customHeight="1">
       <c r="A2" s="5" t="s">
         <v>0</v>
       </c>
@@ -55125,7 +55131,7 @@
         <v>2005</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="10.35" customHeight="1">
+    <row r="3" spans="1:12" ht="10.4" customHeight="1">
       <c r="A3" s="1"/>
       <c r="B3" s="10"/>
       <c r="C3" s="9"/>
@@ -56049,7 +56055,7 @@
       <c r="I33" s="26"/>
       <c r="L33" s="22"/>
     </row>
-    <row r="34" spans="1:12" ht="9.6" customHeight="1">
+    <row r="34" spans="1:12" ht="9.65" customHeight="1">
       <c r="A34" s="1" t="s">
         <v>25</v>
       </c>
@@ -56169,7 +56175,7 @@
       <c r="I37" s="26"/>
       <c r="L37" s="22"/>
     </row>
-    <row r="38" spans="1:12" ht="9.6" customHeight="1">
+    <row r="38" spans="1:12" ht="9.65" customHeight="1">
       <c r="A38" s="1" t="s">
         <v>467</v>
       </c>
@@ -56325,7 +56331,7 @@
       <c r="I42" s="26"/>
       <c r="L42" s="22"/>
     </row>
-    <row r="43" spans="1:12" ht="9.6" customHeight="1">
+    <row r="43" spans="1:12" ht="9.65" customHeight="1">
       <c r="A43" s="1" t="s">
         <v>26</v>
       </c>
@@ -56997,7 +57003,7 @@
       </c>
       <c r="L64" s="22"/>
     </row>
-    <row r="65" spans="1:12" ht="9.6" customHeight="1">
+    <row r="65" spans="1:12" ht="9.65" customHeight="1">
       <c r="A65" s="1" t="s">
         <v>33</v>
       </c>
@@ -57033,7 +57039,7 @@
       </c>
       <c r="L65" s="22"/>
     </row>
-    <row r="66" spans="1:12" ht="9.6" customHeight="1">
+    <row r="66" spans="1:12" ht="9.65" customHeight="1">
       <c r="A66" s="1" t="s">
         <v>34</v>
       </c>
@@ -57069,7 +57075,7 @@
       </c>
       <c r="L66" s="22"/>
     </row>
-    <row r="67" spans="1:12" ht="9.6" customHeight="1">
+    <row r="67" spans="1:12" ht="9.65" customHeight="1">
       <c r="A67" s="1" t="s">
         <v>35</v>
       </c>
@@ -57105,7 +57111,7 @@
       </c>
       <c r="L67" s="22"/>
     </row>
-    <row r="68" spans="1:12" ht="9.6" customHeight="1">
+    <row r="68" spans="1:12" ht="9.65" customHeight="1">
       <c r="A68" s="1" t="s">
         <v>36</v>
       </c>
@@ -57141,7 +57147,7 @@
       </c>
       <c r="L68" s="22"/>
     </row>
-    <row r="69" spans="1:12" ht="9.6" customHeight="1">
+    <row r="69" spans="1:12" ht="9.65" customHeight="1">
       <c r="A69" s="1" t="s">
         <v>37</v>
       </c>
@@ -57189,7 +57195,7 @@
       <c r="I70" s="26"/>
       <c r="L70" s="22"/>
     </row>
-    <row r="71" spans="1:12" ht="9.6" customHeight="1">
+    <row r="71" spans="1:12" ht="9.65" customHeight="1">
       <c r="A71" s="1" t="s">
         <v>413</v>
       </c>
@@ -57417,7 +57423,7 @@
       <c r="I77" s="26"/>
       <c r="L77" s="22"/>
     </row>
-    <row r="78" spans="1:12" ht="9.6" customHeight="1">
+    <row r="78" spans="1:12" ht="9.65" customHeight="1">
       <c r="A78" s="1" t="s">
         <v>361</v>
       </c>
@@ -57561,7 +57567,7 @@
       </c>
       <c r="L81" s="22"/>
     </row>
-    <row r="82" spans="1:12" ht="9.6" customHeight="1">
+    <row r="82" spans="1:12" ht="9.65" customHeight="1">
       <c r="A82" s="1" t="s">
         <v>362</v>
       </c>
@@ -57717,7 +57723,7 @@
       </c>
       <c r="L86" s="22"/>
     </row>
-    <row r="87" spans="1:12" ht="10.35" customHeight="1">
+    <row r="87" spans="1:12" ht="10.4" customHeight="1">
       <c r="A87" s="16" t="s">
         <v>49</v>
       </c>
@@ -57753,7 +57759,7 @@
       </c>
       <c r="L87" s="22"/>
     </row>
-    <row r="88" spans="1:12" ht="10.35" customHeight="1">
+    <row r="88" spans="1:12" ht="10.4" customHeight="1">
       <c r="A88" s="29"/>
       <c r="B88" s="30"/>
       <c r="C88" s="31"/>
@@ -57763,13 +57769,13 @@
         <v>60</v>
       </c>
     </row>
-    <row r="89" spans="1:12" ht="10.35" customHeight="1">
+    <row r="89" spans="1:12" ht="10.4" customHeight="1">
       <c r="A89" s="1"/>
       <c r="B89" s="30"/>
       <c r="C89" s="31"/>
       <c r="D89" s="31"/>
     </row>
-    <row r="90" spans="1:12" ht="10.35" customHeight="1">
+    <row r="90" spans="1:12" ht="10.4" customHeight="1">
       <c r="A90" s="1"/>
       <c r="B90" s="30"/>
       <c r="C90" s="30"/>
@@ -57782,7 +57788,7 @@
       <c r="J90" s="30"/>
       <c r="K90" s="30"/>
     </row>
-    <row r="91" spans="1:12" ht="10.35" customHeight="1">
+    <row r="91" spans="1:12" ht="10.4" customHeight="1">
       <c r="B91" s="30"/>
       <c r="C91" s="30"/>
       <c r="D91" s="30"/>
@@ -57792,7 +57798,7 @@
       <c r="H91" s="30"/>
       <c r="I91" s="30"/>
     </row>
-    <row r="92" spans="1:12" ht="10.35" customHeight="1">
+    <row r="92" spans="1:12" ht="10.4" customHeight="1">
       <c r="A92" s="1"/>
       <c r="B92" s="30"/>
       <c r="C92" s="30"/>
@@ -57805,7 +57811,7 @@
       <c r="J92" s="18"/>
       <c r="K92" s="18"/>
     </row>
-    <row r="93" spans="1:12" ht="10.35" customHeight="1">
+    <row r="93" spans="1:12" ht="10.4" customHeight="1">
       <c r="A93" s="1"/>
       <c r="B93" s="30"/>
       <c r="C93" s="31"/>
@@ -57866,20 +57872,20 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <sheetPr transitionEvaluation="1"/>
   <dimension ref="A1:L100"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="120" zoomScaleNormal="120" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="13.42578125" defaultRowHeight="9"/>
+  <sheetFormatPr defaultColWidth="13.453125" defaultRowHeight="9"/>
   <cols>
     <col min="1" max="1" width="22" style="17" customWidth="1"/>
-    <col min="2" max="11" width="9.140625" style="17" customWidth="1"/>
-    <col min="12" max="16384" width="13.42578125" style="17"/>
+    <col min="2" max="11" width="9.1796875" style="17" customWidth="1"/>
+    <col min="12" max="16384" width="13.453125" style="17"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="10.35" customHeight="1">
+    <row r="1" spans="1:12" ht="10.4" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>468</v>
       </c>
@@ -57894,7 +57900,7 @@
       <c r="J1" s="1"/>
       <c r="K1" s="1"/>
     </row>
-    <row r="2" spans="1:12" ht="10.35" customHeight="1">
+    <row r="2" spans="1:12" ht="10.4" customHeight="1">
       <c r="A2" s="5" t="s">
         <v>0</v>
       </c>
@@ -57929,7 +57935,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="10.35" customHeight="1">
+    <row r="3" spans="1:12" ht="10.4" customHeight="1">
       <c r="A3" s="1"/>
       <c r="E3" s="8" t="s">
         <v>412</v>
@@ -59664,7 +59670,7 @@
       <c r="I63" s="18"/>
       <c r="J63" s="22"/>
     </row>
-    <row r="64" spans="1:11" ht="8.85" customHeight="1">
+    <row r="64" spans="1:11" ht="8.9" customHeight="1">
       <c r="A64" s="1" t="s">
         <v>32</v>
       </c>
@@ -60103,7 +60109,7 @@
       <c r="H77" s="18"/>
       <c r="I77" s="18"/>
     </row>
-    <row r="78" spans="1:11" ht="9.6" customHeight="1">
+    <row r="78" spans="1:11" ht="9.65" customHeight="1">
       <c r="A78" s="1" t="s">
         <v>361</v>
       </c>
@@ -60243,7 +60249,7 @@
         <v>0.39451315908944129</v>
       </c>
     </row>
-    <row r="82" spans="1:11" ht="9.6" customHeight="1">
+    <row r="82" spans="1:11" ht="9.65" customHeight="1">
       <c r="A82" s="1" t="s">
         <v>362</v>
       </c>
@@ -60390,7 +60396,7 @@
         <v>190.70957797138564</v>
       </c>
     </row>
-    <row r="87" spans="1:11" ht="8.85" customHeight="1">
+    <row r="87" spans="1:11" ht="8.9" customHeight="1">
       <c r="A87" s="16" t="s">
         <v>49</v>
       </c>
@@ -60425,7 +60431,7 @@
         <v>24.003079194100938</v>
       </c>
     </row>
-    <row r="88" spans="1:11" ht="11.1" customHeight="1">
+    <row r="88" spans="1:11" ht="11.15" customHeight="1">
       <c r="B88"/>
       <c r="C88"/>
       <c r="D88"/>
@@ -60504,7 +60510,7 @@
       <c r="J93"/>
       <c r="K93"/>
     </row>
-    <row r="94" spans="1:11" ht="11.1" customHeight="1">
+    <row r="94" spans="1:11" ht="11.15" customHeight="1">
       <c r="A94" s="1"/>
       <c r="B94"/>
       <c r="C94"/>
@@ -60517,7 +60523,7 @@
       <c r="J94"/>
       <c r="K94"/>
     </row>
-    <row r="95" spans="1:11" ht="11.1" customHeight="1">
+    <row r="95" spans="1:11" ht="11.15" customHeight="1">
       <c r="A95" s="1"/>
       <c r="B95" s="41"/>
       <c r="C95" s="41"/>
@@ -60530,7 +60536,7 @@
       <c r="J95"/>
       <c r="K95"/>
     </row>
-    <row r="96" spans="1:11" ht="11.1" customHeight="1">
+    <row r="96" spans="1:11" ht="11.15" customHeight="1">
       <c r="B96" s="39"/>
       <c r="C96" s="39"/>
       <c r="D96" s="39"/>
@@ -60542,7 +60548,7 @@
       <c r="J96"/>
       <c r="K96"/>
     </row>
-    <row r="97" spans="2:11" ht="15">
+    <row r="97" spans="2:11" ht="14.5">
       <c r="B97" s="39"/>
       <c r="C97" s="39"/>
       <c r="D97" s="39"/>
@@ -60593,22 +60599,22 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <sheetPr transitionEvaluation="1"/>
   <dimension ref="A1:E98"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A93" sqref="A93"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="13.42578125" defaultRowHeight="9"/>
+  <sheetFormatPr defaultColWidth="13.453125" defaultRowHeight="9"/>
   <cols>
     <col min="1" max="1" width="22" style="17" customWidth="1"/>
-    <col min="2" max="4" width="20.7109375" style="17" customWidth="1"/>
-    <col min="5" max="16384" width="13.42578125" style="17"/>
+    <col min="2" max="4" width="20.7265625" style="17" customWidth="1"/>
+    <col min="5" max="16384" width="13.453125" style="17"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="10.35" customHeight="1">
+    <row r="1" spans="1:5" ht="10.4" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>468</v>
       </c>
@@ -60616,7 +60622,7 @@
       <c r="C1" s="525"/>
       <c r="D1" s="525"/>
     </row>
-    <row r="2" spans="1:5" ht="10.35" customHeight="1">
+    <row r="2" spans="1:5" ht="10.4" customHeight="1">
       <c r="A2" s="5" t="s">
         <v>0</v>
       </c>
@@ -60630,7 +60636,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="10.35" customHeight="1">
+    <row r="3" spans="1:5" ht="10.4" customHeight="1">
       <c r="A3" s="1"/>
       <c r="B3" s="527"/>
       <c r="C3" s="8" t="s">
@@ -60816,8 +60822,8 @@
       <c r="C17" s="33">
         <v>5.8556440627009874</v>
       </c>
-      <c r="D17" s="536" t="s">
-        <v>469</v>
+      <c r="D17" s="536">
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="8.65" customHeight="1">
@@ -61348,7 +61354,7 @@
       <c r="A63" s="1"/>
       <c r="B63" s="527"/>
     </row>
-    <row r="64" spans="1:4" ht="8.85" customHeight="1">
+    <row r="64" spans="1:4" ht="8.9" customHeight="1">
       <c r="A64" s="1" t="s">
         <v>32</v>
       </c>
@@ -61524,7 +61530,7 @@
       <c r="A77" s="1"/>
       <c r="B77" s="527"/>
     </row>
-    <row r="78" spans="1:4" ht="9.6" customHeight="1">
+    <row r="78" spans="1:4" ht="9.65" customHeight="1">
       <c r="A78" s="1" t="s">
         <v>361</v>
       </c>
@@ -61580,7 +61586,7 @@
         <v>0.53953859854119079</v>
       </c>
     </row>
-    <row r="82" spans="1:4" ht="9.6" customHeight="1">
+    <row r="82" spans="1:4" ht="9.65" customHeight="1">
       <c r="A82" s="1" t="s">
         <v>362</v>
       </c>
@@ -61640,7 +61646,7 @@
         <v>182.95540620510087</v>
       </c>
     </row>
-    <row r="87" spans="1:4" ht="8.85" customHeight="1">
+    <row r="87" spans="1:4" ht="8.9" customHeight="1">
       <c r="A87" s="16" t="s">
         <v>49</v>
       </c>
@@ -61654,19 +61660,19 @@
         <v>25.194260644670557</v>
       </c>
     </row>
-    <row r="88" spans="1:4" ht="11.1" customHeight="1">
+    <row r="88" spans="1:4" ht="11.15" customHeight="1">
       <c r="A88" s="17" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
     </row>
     <row r="89" spans="1:4" ht="11.25" customHeight="1">
       <c r="A89" s="40" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="90" spans="1:4" ht="11.25" customHeight="1">
       <c r="A90" s="29" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
     </row>
     <row r="91" spans="1:4" ht="11.25" customHeight="1">
@@ -61676,7 +61682,7 @@
     </row>
     <row r="92" spans="1:4" ht="11.25" customHeight="1">
       <c r="A92" s="40" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
     </row>
     <row r="93" spans="1:4" ht="11.25" customHeight="1">
@@ -61684,17 +61690,17 @@
         <v>69</v>
       </c>
     </row>
-    <row r="94" spans="1:4" ht="11.1" customHeight="1">
+    <row r="94" spans="1:4" ht="11.15" customHeight="1">
       <c r="A94" s="1" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="95" spans="1:4" ht="11.1" customHeight="1">
+    <row r="95" spans="1:4" ht="11.15" customHeight="1">
       <c r="A95" s="1" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="96" spans="1:4" ht="11.1" customHeight="1">
+    <row r="96" spans="1:4" ht="11.15" customHeight="1">
       <c r="A96" s="17" t="s">
         <v>72</v>
       </c>
@@ -61712,7 +61718,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -61725,14 +61731,14 @@
       <selection pane="bottomRight" activeCell="N39" sqref="N39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="11.5"/>
   <cols>
-    <col min="1" max="1" width="13.42578125" style="44" customWidth="1"/>
-    <col min="2" max="6" width="17.5703125" style="44" customWidth="1"/>
-    <col min="7" max="7" width="9.85546875" style="44" bestFit="1" customWidth="1"/>
-    <col min="8" max="10" width="9.140625" style="44"/>
-    <col min="11" max="11" width="13.5703125" style="44" bestFit="1" customWidth="1"/>
-    <col min="12" max="16384" width="9.140625" style="44"/>
+    <col min="1" max="1" width="13.453125" style="44" customWidth="1"/>
+    <col min="2" max="6" width="17.54296875" style="44" customWidth="1"/>
+    <col min="7" max="7" width="9.81640625" style="44" bestFit="1" customWidth="1"/>
+    <col min="8" max="10" width="9.1796875" style="44"/>
+    <col min="11" max="11" width="13.54296875" style="44" bestFit="1" customWidth="1"/>
+    <col min="12" max="16384" width="9.1796875" style="44"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="12" customHeight="1">
@@ -61745,7 +61751,7 @@
       <c r="E1" s="43"/>
       <c r="F1" s="43"/>
     </row>
-    <row r="2" spans="1:7" ht="6.95" customHeight="1">
+    <row r="2" spans="1:7" ht="7" customHeight="1">
       <c r="A2" s="45"/>
       <c r="B2" s="46"/>
       <c r="C2" s="46"/>
@@ -61761,7 +61767,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" ht="12.5">
       <c r="A4" s="48" t="s">
         <v>76</v>
       </c>
@@ -61782,7 +61788,7 @@
       </c>
       <c r="G4" s="50"/>
     </row>
-    <row r="5" spans="1:7" ht="5.0999999999999996" customHeight="1">
+    <row r="5" spans="1:7" ht="5.15" customHeight="1">
       <c r="A5" s="51"/>
       <c r="B5" s="52"/>
       <c r="C5" s="52"/>
@@ -62766,70 +62772,70 @@
       <c r="E57" s="60"/>
       <c r="F57" s="60"/>
     </row>
-    <row r="58" spans="1:11" ht="15">
+    <row r="58" spans="1:11" ht="14.5">
       <c r="A58"/>
       <c r="B58"/>
       <c r="C58"/>
       <c r="D58"/>
       <c r="E58"/>
     </row>
-    <row r="59" spans="1:11" ht="15">
+    <row r="59" spans="1:11" ht="14.5">
       <c r="A59"/>
       <c r="B59"/>
       <c r="C59"/>
       <c r="D59"/>
       <c r="E59"/>
     </row>
-    <row r="60" spans="1:11" ht="15">
+    <row r="60" spans="1:11" ht="14.5">
       <c r="A60"/>
       <c r="B60"/>
       <c r="C60"/>
       <c r="D60"/>
       <c r="E60"/>
     </row>
-    <row r="61" spans="1:11" ht="15">
+    <row r="61" spans="1:11" ht="14.5">
       <c r="A61"/>
       <c r="B61"/>
       <c r="C61"/>
       <c r="D61"/>
       <c r="E61"/>
     </row>
-    <row r="62" spans="1:11" ht="15">
+    <row r="62" spans="1:11" ht="14.5">
       <c r="A62"/>
       <c r="B62"/>
       <c r="C62"/>
       <c r="D62"/>
       <c r="E62"/>
     </row>
-    <row r="63" spans="1:11" ht="15">
+    <row r="63" spans="1:11" ht="14.5">
       <c r="A63"/>
       <c r="B63"/>
       <c r="C63"/>
       <c r="D63"/>
       <c r="E63"/>
     </row>
-    <row r="64" spans="1:11" ht="15">
+    <row r="64" spans="1:11" ht="14.5">
       <c r="A64"/>
       <c r="B64"/>
       <c r="C64"/>
       <c r="D64"/>
       <c r="E64"/>
     </row>
-    <row r="65" spans="1:6" ht="15">
+    <row r="65" spans="1:6" ht="14.5">
       <c r="A65"/>
       <c r="B65"/>
       <c r="C65"/>
       <c r="D65"/>
       <c r="E65"/>
     </row>
-    <row r="66" spans="1:6" ht="15">
+    <row r="66" spans="1:6" ht="14.5">
       <c r="A66"/>
       <c r="B66"/>
       <c r="C66"/>
       <c r="D66"/>
       <c r="E66"/>
     </row>
-    <row r="67" spans="1:6" ht="15">
+    <row r="67" spans="1:6" ht="14.5">
       <c r="A67"/>
       <c r="B67"/>
       <c r="C67"/>
@@ -62854,33 +62860,33 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <sheetPr transitionEvaluation="1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:AF58"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="6" topLeftCell="B7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
       <selection pane="bottomRight" activeCell="J47" sqref="J47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.7109375" defaultRowHeight="12"/>
+  <sheetFormatPr defaultColWidth="9.7265625" defaultRowHeight="11.5"/>
   <cols>
-    <col min="1" max="1" width="7.5703125" style="44" customWidth="1"/>
-    <col min="2" max="3" width="10.5703125" style="44" customWidth="1"/>
-    <col min="4" max="5" width="11.5703125" style="44" customWidth="1"/>
-    <col min="6" max="6" width="1.7109375" style="44" customWidth="1"/>
-    <col min="7" max="7" width="11.5703125" style="44" customWidth="1"/>
-    <col min="8" max="9" width="12.7109375" style="44" customWidth="1"/>
-    <col min="10" max="10" width="11.5703125" style="44" customWidth="1"/>
-    <col min="11" max="11" width="17.28515625" style="44" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.140625" style="44" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.7109375" style="44"/>
+    <col min="1" max="1" width="7.54296875" style="44" customWidth="1"/>
+    <col min="2" max="3" width="10.54296875" style="44" customWidth="1"/>
+    <col min="4" max="5" width="11.54296875" style="44" customWidth="1"/>
+    <col min="6" max="6" width="1.7265625" style="44" customWidth="1"/>
+    <col min="7" max="7" width="11.54296875" style="44" customWidth="1"/>
+    <col min="8" max="9" width="12.7265625" style="44" customWidth="1"/>
+    <col min="10" max="10" width="11.54296875" style="44" customWidth="1"/>
+    <col min="11" max="11" width="17.26953125" style="44" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.1796875" style="44" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.7265625" style="44"/>
     <col min="14" max="14" width="11" style="44" bestFit="1" customWidth="1"/>
-    <col min="15" max="16384" width="9.7109375" style="44"/>
+    <col min="15" max="16384" width="9.7265625" style="44"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:32" ht="10.5" customHeight="1">
@@ -62897,7 +62903,7 @@
       <c r="I1" s="71"/>
       <c r="J1" s="71"/>
     </row>
-    <row r="2" spans="1:32" ht="5.0999999999999996" customHeight="1">
+    <row r="2" spans="1:32" ht="5.15" customHeight="1">
       <c r="A2" s="45"/>
       <c r="B2" s="46"/>
       <c r="C2" s="46"/>
@@ -62925,7 +62931,7 @@
       <c r="I3" s="73"/>
       <c r="J3" s="72"/>
     </row>
-    <row r="4" spans="1:32" ht="5.0999999999999996" customHeight="1">
+    <row r="4" spans="1:32" ht="5.15" customHeight="1">
       <c r="A4" s="53"/>
       <c r="B4" s="74"/>
       <c r="C4" s="75"/>
@@ -62967,7 +62973,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="6" spans="1:32" ht="5.0999999999999996" customHeight="1">
+    <row r="6" spans="1:32" ht="5.15" customHeight="1">
       <c r="A6" s="51"/>
       <c r="B6" s="52"/>
       <c r="C6" s="52"/>
@@ -64096,7 +64102,7 @@
       <c r="M40" s="488"/>
       <c r="N40" s="100"/>
     </row>
-    <row r="41" spans="1:14" ht="12.95" customHeight="1">
+    <row r="41" spans="1:14" ht="13" customHeight="1">
       <c r="A41" s="97" t="s">
         <v>98</v>
       </c>
@@ -64306,7 +64312,7 @@
       <c r="L46" s="486"/>
       <c r="M46" s="488"/>
     </row>
-    <row r="47" spans="1:14" ht="12.95" customHeight="1">
+    <row r="47" spans="1:14" ht="13" customHeight="1">
       <c r="A47" s="101" t="s">
         <v>454</v>
       </c>
@@ -64460,7 +64466,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <sheetPr transitionEvaluation="1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -64470,10 +64476,10 @@
       <selection activeCell="O99" sqref="O99"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.7109375" defaultRowHeight="12"/>
+  <sheetFormatPr defaultColWidth="9.7265625" defaultRowHeight="11.5"/>
   <cols>
-    <col min="1" max="15" width="9.140625" style="160" customWidth="1"/>
-    <col min="16" max="16384" width="9.7109375" style="160"/>
+    <col min="1" max="15" width="9.1796875" style="160" customWidth="1"/>
+    <col min="16" max="16384" width="9.7265625" style="160"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" s="111" customFormat="1" ht="10.15" customHeight="1">
@@ -64495,7 +64501,7 @@
       <c r="N1" s="109"/>
       <c r="O1" s="109"/>
     </row>
-    <row r="2" spans="1:15" s="111" customFormat="1" ht="3.95" customHeight="1">
+    <row r="2" spans="1:15" s="111" customFormat="1" ht="4" customHeight="1">
       <c r="A2" s="112"/>
       <c r="B2" s="113"/>
       <c r="C2" s="113"/>
@@ -64545,7 +64551,7 @@
       </c>
       <c r="N4" s="117"/>
     </row>
-    <row r="5" spans="1:15" s="111" customFormat="1" ht="12.95" customHeight="1">
+    <row r="5" spans="1:15" s="111" customFormat="1" ht="13" customHeight="1">
       <c r="A5" s="119" t="s">
         <v>107</v>
       </c>
@@ -64592,7 +64598,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="6" spans="1:15" s="111" customFormat="1" ht="3.95" customHeight="1">
+    <row r="6" spans="1:15" s="111" customFormat="1" ht="4" customHeight="1">
       <c r="A6" s="119"/>
       <c r="B6" s="118"/>
       <c r="C6" s="118"/>
@@ -65746,7 +65752,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="32" spans="1:16" s="111" customFormat="1" ht="12.95" customHeight="1">
+    <row r="32" spans="1:16" s="111" customFormat="1" ht="13" customHeight="1">
       <c r="A32" s="112" t="s">
         <v>83</v>
       </c>
@@ -65794,7 +65800,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="33" spans="1:22" s="111" customFormat="1" ht="12.95" customHeight="1">
+    <row r="33" spans="1:22" s="111" customFormat="1" ht="13" customHeight="1">
       <c r="A33" s="112" t="s">
         <v>84</v>
       </c>
@@ -65842,7 +65848,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="34" spans="1:22" s="111" customFormat="1" ht="12.95" customHeight="1">
+    <row r="34" spans="1:22" s="111" customFormat="1" ht="13" customHeight="1">
       <c r="A34" s="112">
         <v>2005</v>
       </c>
@@ -65890,7 +65896,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="35" spans="1:22" s="111" customFormat="1" ht="12.95" customHeight="1">
+    <row r="35" spans="1:22" s="111" customFormat="1" ht="13" customHeight="1">
       <c r="A35" s="112">
         <v>2006</v>
       </c>
@@ -65938,7 +65944,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="36" spans="1:22" s="111" customFormat="1" ht="12.95" customHeight="1">
+    <row r="36" spans="1:22" s="111" customFormat="1" ht="13" customHeight="1">
       <c r="A36" s="112">
         <v>2007</v>
       </c>
@@ -65990,7 +65996,7 @@
       <c r="U36" s="381"/>
       <c r="V36" s="381"/>
     </row>
-    <row r="37" spans="1:22" s="111" customFormat="1" ht="12.95" customHeight="1">
+    <row r="37" spans="1:22" s="111" customFormat="1" ht="13" customHeight="1">
       <c r="A37" s="112">
         <v>2008</v>
       </c>
@@ -66042,7 +66048,7 @@
       <c r="U37" s="381"/>
       <c r="V37" s="381"/>
     </row>
-    <row r="38" spans="1:22" s="111" customFormat="1" ht="12.95" customHeight="1">
+    <row r="38" spans="1:22" s="111" customFormat="1" ht="13" customHeight="1">
       <c r="A38" s="112">
         <v>2009</v>
       </c>
@@ -66094,7 +66100,7 @@
       <c r="U38" s="381"/>
       <c r="V38" s="381"/>
     </row>
-    <row r="39" spans="1:22" s="111" customFormat="1" ht="12.95" customHeight="1">
+    <row r="39" spans="1:22" s="111" customFormat="1" ht="13" customHeight="1">
       <c r="A39" s="112">
         <v>2010</v>
       </c>
@@ -66146,7 +66152,7 @@
       <c r="U39" s="381"/>
       <c r="V39" s="381"/>
     </row>
-    <row r="40" spans="1:22" s="111" customFormat="1" ht="12.95" customHeight="1">
+    <row r="40" spans="1:22" s="111" customFormat="1" ht="13" customHeight="1">
       <c r="A40" s="112">
         <v>2011</v>
       </c>
@@ -66198,7 +66204,7 @@
       <c r="U40" s="381"/>
       <c r="V40" s="381"/>
     </row>
-    <row r="41" spans="1:22" s="111" customFormat="1" ht="12.95" customHeight="1">
+    <row r="41" spans="1:22" s="111" customFormat="1" ht="13" customHeight="1">
       <c r="A41" s="112" t="s">
         <v>85</v>
       </c>
@@ -66250,7 +66256,7 @@
       <c r="U41" s="381"/>
       <c r="V41" s="381"/>
     </row>
-    <row r="42" spans="1:22" s="111" customFormat="1" ht="12.95" customHeight="1">
+    <row r="42" spans="1:22" s="111" customFormat="1" ht="13" customHeight="1">
       <c r="A42" s="112" t="s">
         <v>86</v>
       </c>
@@ -66302,7 +66308,7 @@
       <c r="U42" s="381"/>
       <c r="V42" s="381"/>
     </row>
-    <row r="43" spans="1:22" s="111" customFormat="1" ht="12.95" customHeight="1">
+    <row r="43" spans="1:22" s="111" customFormat="1" ht="13" customHeight="1">
       <c r="A43" s="112">
         <v>2014</v>
       </c>
@@ -66354,7 +66360,7 @@
       <c r="U43" s="381"/>
       <c r="V43" s="381"/>
     </row>
-    <row r="44" spans="1:22" s="111" customFormat="1" ht="12.95" customHeight="1">
+    <row r="44" spans="1:22" s="111" customFormat="1" ht="13" customHeight="1">
       <c r="A44" s="112">
         <v>2015</v>
       </c>
@@ -66407,7 +66413,7 @@
       <c r="U44" s="381"/>
       <c r="V44" s="381"/>
     </row>
-    <row r="45" spans="1:22" s="111" customFormat="1" ht="12.95" customHeight="1">
+    <row r="45" spans="1:22" s="111" customFormat="1" ht="13" customHeight="1">
       <c r="A45" s="112">
         <v>2016</v>
       </c>
@@ -66463,7 +66469,7 @@
       <c r="U45" s="381"/>
       <c r="V45" s="381"/>
     </row>
-    <row r="46" spans="1:22" s="111" customFormat="1" ht="12.95" customHeight="1">
+    <row r="46" spans="1:22" s="111" customFormat="1" ht="13" customHeight="1">
       <c r="A46" s="112">
         <v>2017</v>
       </c>
@@ -66519,7 +66525,7 @@
       <c r="U46" s="381"/>
       <c r="V46" s="381"/>
     </row>
-    <row r="47" spans="1:22" s="111" customFormat="1" ht="12.95" customHeight="1">
+    <row r="47" spans="1:22" s="111" customFormat="1" ht="13" customHeight="1">
       <c r="A47" s="112">
         <v>2018</v>
       </c>
@@ -66572,7 +66578,7 @@
       <c r="U47" s="381"/>
       <c r="V47" s="381"/>
     </row>
-    <row r="48" spans="1:22" s="111" customFormat="1" ht="3.95" customHeight="1">
+    <row r="48" spans="1:22" s="111" customFormat="1" ht="4" customHeight="1">
       <c r="A48" s="112"/>
       <c r="B48" s="132"/>
       <c r="C48" s="132"/>
@@ -66589,7 +66595,7 @@
       <c r="N48" s="134"/>
       <c r="O48" s="137"/>
     </row>
-    <row r="49" spans="1:15" s="111" customFormat="1" ht="11.1" customHeight="1">
+    <row r="49" spans="1:15" s="111" customFormat="1" ht="11.15" customHeight="1">
       <c r="A49" s="114"/>
       <c r="B49" s="117" t="s">
         <v>123</v>
@@ -66616,7 +66622,7 @@
       <c r="N49" s="117"/>
       <c r="O49" s="117"/>
     </row>
-    <row r="50" spans="1:15" s="111" customFormat="1" ht="12.95" customHeight="1">
+    <row r="50" spans="1:15" s="111" customFormat="1" ht="13" customHeight="1">
       <c r="A50" s="119" t="s">
         <v>107</v>
       </c>
@@ -66663,7 +66669,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="51" spans="1:15" s="111" customFormat="1" ht="3.95" customHeight="1">
+    <row r="51" spans="1:15" s="111" customFormat="1" ht="4" customHeight="1">
       <c r="A51" s="119"/>
       <c r="B51" s="118"/>
       <c r="C51" s="118"/>
@@ -67196,7 +67202,7 @@
         <v>2792.08</v>
       </c>
     </row>
-    <row r="64" spans="1:15" s="111" customFormat="1" ht="12.95" customHeight="1">
+    <row r="64" spans="1:15" s="111" customFormat="1" ht="13" customHeight="1">
       <c r="A64" s="119" t="s">
         <v>55</v>
       </c>
@@ -67243,7 +67249,7 @@
         <v>2784.3</v>
       </c>
     </row>
-    <row r="65" spans="1:16" s="111" customFormat="1" ht="12.95" customHeight="1">
+    <row r="65" spans="1:16" s="111" customFormat="1" ht="13" customHeight="1">
       <c r="A65" s="119" t="s">
         <v>56</v>
       </c>
@@ -67291,7 +67297,7 @@
         <v>2770.9249999999993</v>
       </c>
     </row>
-    <row r="66" spans="1:16" s="111" customFormat="1" ht="12.95" customHeight="1">
+    <row r="66" spans="1:16" s="111" customFormat="1" ht="13" customHeight="1">
       <c r="A66" s="119" t="s">
         <v>57</v>
       </c>
@@ -67340,7 +67346,7 @@
       </c>
       <c r="P66" s="143"/>
     </row>
-    <row r="67" spans="1:16" s="111" customFormat="1" ht="12.95" customHeight="1">
+    <row r="67" spans="1:16" s="111" customFormat="1" ht="13" customHeight="1">
       <c r="A67" s="119" t="s">
         <v>58</v>
       </c>
@@ -67389,7 +67395,7 @@
       </c>
       <c r="P67" s="126"/>
     </row>
-    <row r="68" spans="1:16" s="111" customFormat="1" ht="12.95" customHeight="1">
+    <row r="68" spans="1:16" s="111" customFormat="1" ht="13" customHeight="1">
       <c r="A68" s="119" t="s">
         <v>59</v>
       </c>
@@ -67437,7 +67443,7 @@
         <v>2934.9199999999996</v>
       </c>
     </row>
-    <row r="69" spans="1:16" s="111" customFormat="1" ht="12.95" customHeight="1">
+    <row r="69" spans="1:16" s="111" customFormat="1" ht="13" customHeight="1">
       <c r="A69" s="128" t="s">
         <v>122</v>
       </c>
@@ -67485,7 +67491,7 @@
         <v>3015.2650000000003</v>
       </c>
     </row>
-    <row r="70" spans="1:16" s="111" customFormat="1" ht="12.95" customHeight="1">
+    <row r="70" spans="1:16" s="111" customFormat="1" ht="13" customHeight="1">
       <c r="A70" s="128">
         <v>1996</v>
       </c>
@@ -67533,7 +67539,7 @@
         <v>3098.1</v>
       </c>
     </row>
-    <row r="71" spans="1:16" s="111" customFormat="1" ht="12.95" customHeight="1">
+    <row r="71" spans="1:16" s="111" customFormat="1" ht="13" customHeight="1">
       <c r="A71" s="128">
         <v>1997</v>
       </c>
@@ -67581,7 +67587,7 @@
         <v>3159.7849999999999</v>
       </c>
     </row>
-    <row r="72" spans="1:16" s="111" customFormat="1" ht="12.95" customHeight="1">
+    <row r="72" spans="1:16" s="111" customFormat="1" ht="13" customHeight="1">
       <c r="A72" s="128">
         <v>1998</v>
       </c>
@@ -67629,7 +67635,7 @@
         <v>3158.5299999999997</v>
       </c>
     </row>
-    <row r="73" spans="1:16" s="111" customFormat="1" ht="12.95" customHeight="1">
+    <row r="73" spans="1:16" s="111" customFormat="1" ht="13" customHeight="1">
       <c r="A73" s="128">
         <v>1999</v>
       </c>
@@ -67677,7 +67683,7 @@
         <v>3181.3100000000004</v>
       </c>
     </row>
-    <row r="74" spans="1:16" s="111" customFormat="1" ht="12.95" customHeight="1">
+    <row r="74" spans="1:16" s="111" customFormat="1" ht="13" customHeight="1">
       <c r="A74" s="112" t="s">
         <v>65</v>
       </c>
@@ -67726,7 +67732,7 @@
       </c>
       <c r="P74" s="145"/>
     </row>
-    <row r="75" spans="1:16" s="111" customFormat="1" ht="12.95" customHeight="1">
+    <row r="75" spans="1:16" s="111" customFormat="1" ht="13" customHeight="1">
       <c r="A75" s="112" t="s">
         <v>66</v>
       </c>
@@ -67775,7 +67781,7 @@
       </c>
       <c r="P75" s="145"/>
     </row>
-    <row r="76" spans="1:16" s="111" customFormat="1" ht="12.95" customHeight="1">
+    <row r="76" spans="1:16" s="111" customFormat="1" ht="13" customHeight="1">
       <c r="A76" s="112" t="s">
         <v>67</v>
       </c>
@@ -67824,7 +67830,7 @@
       </c>
       <c r="P76" s="145"/>
     </row>
-    <row r="77" spans="1:16" s="111" customFormat="1" ht="12.95" customHeight="1">
+    <row r="77" spans="1:16" s="111" customFormat="1" ht="13" customHeight="1">
       <c r="A77" s="112" t="s">
         <v>83</v>
       </c>
@@ -67873,7 +67879,7 @@
       </c>
       <c r="P77" s="145"/>
     </row>
-    <row r="78" spans="1:16" s="111" customFormat="1" ht="12.95" customHeight="1">
+    <row r="78" spans="1:16" s="111" customFormat="1" ht="13" customHeight="1">
       <c r="A78" s="112" t="s">
         <v>84</v>
       </c>
@@ -67922,7 +67928,7 @@
       </c>
       <c r="P78" s="145"/>
     </row>
-    <row r="79" spans="1:16" s="111" customFormat="1" ht="12.95" customHeight="1">
+    <row r="79" spans="1:16" s="111" customFormat="1" ht="13" customHeight="1">
       <c r="A79" s="112">
         <v>2005</v>
       </c>
@@ -67971,7 +67977,7 @@
       </c>
       <c r="P79" s="145"/>
     </row>
-    <row r="80" spans="1:16" s="111" customFormat="1" ht="12.95" customHeight="1">
+    <row r="80" spans="1:16" s="111" customFormat="1" ht="13" customHeight="1">
       <c r="A80" s="112">
         <v>2006</v>
       </c>
@@ -68020,7 +68026,7 @@
       </c>
       <c r="P80" s="145"/>
     </row>
-    <row r="81" spans="1:24" s="150" customFormat="1" ht="12.95" customHeight="1">
+    <row r="81" spans="1:24" s="150" customFormat="1" ht="13" customHeight="1">
       <c r="A81" s="112">
         <v>2007</v>
       </c>
@@ -68071,7 +68077,7 @@
       <c r="W81" s="381"/>
       <c r="X81" s="111"/>
     </row>
-    <row r="82" spans="1:24" s="111" customFormat="1" ht="12.95" customHeight="1">
+    <row r="82" spans="1:24" s="111" customFormat="1" ht="13" customHeight="1">
       <c r="A82" s="112">
         <v>2008</v>
       </c>
@@ -68121,7 +68127,7 @@
       <c r="P82" s="145"/>
       <c r="W82" s="381"/>
     </row>
-    <row r="83" spans="1:24" s="111" customFormat="1" ht="12.95" customHeight="1">
+    <row r="83" spans="1:24" s="111" customFormat="1" ht="13" customHeight="1">
       <c r="A83" s="112">
         <v>2009</v>
       </c>
@@ -68171,7 +68177,7 @@
       <c r="P83" s="145"/>
       <c r="W83" s="381"/>
     </row>
-    <row r="84" spans="1:24" s="111" customFormat="1" ht="12.95" customHeight="1">
+    <row r="84" spans="1:24" s="111" customFormat="1" ht="13" customHeight="1">
       <c r="A84" s="112">
         <v>2010</v>
       </c>
@@ -68222,7 +68228,7 @@
       <c r="R84" s="494"/>
       <c r="W84" s="381"/>
     </row>
-    <row r="85" spans="1:24" s="111" customFormat="1" ht="12.95" customHeight="1">
+    <row r="85" spans="1:24" s="111" customFormat="1" ht="13" customHeight="1">
       <c r="A85" s="112">
         <v>2011</v>
       </c>
@@ -68273,7 +68279,7 @@
       <c r="R85" s="494"/>
       <c r="W85" s="381"/>
     </row>
-    <row r="86" spans="1:24" s="111" customFormat="1" ht="12.95" customHeight="1">
+    <row r="86" spans="1:24" s="111" customFormat="1" ht="13" customHeight="1">
       <c r="A86" s="112" t="s">
         <v>141</v>
       </c>
@@ -68323,7 +68329,7 @@
       <c r="R86" s="494"/>
       <c r="W86" s="381"/>
     </row>
-    <row r="87" spans="1:24" s="111" customFormat="1" ht="12.95" customHeight="1">
+    <row r="87" spans="1:24" s="111" customFormat="1" ht="13" customHeight="1">
       <c r="A87" s="112" t="s">
         <v>86</v>
       </c>
@@ -68374,7 +68380,7 @@
       <c r="R87" s="494"/>
       <c r="W87" s="381"/>
     </row>
-    <row r="88" spans="1:24" s="111" customFormat="1" ht="12.95" customHeight="1">
+    <row r="88" spans="1:24" s="111" customFormat="1" ht="13" customHeight="1">
       <c r="A88" s="112">
         <v>2014</v>
       </c>
@@ -68425,7 +68431,7 @@
       <c r="R88" s="494"/>
       <c r="W88" s="381"/>
     </row>
-    <row r="89" spans="1:24" s="111" customFormat="1" ht="12.95" customHeight="1">
+    <row r="89" spans="1:24" s="111" customFormat="1" ht="13" customHeight="1">
       <c r="A89" s="112">
         <v>2015</v>
       </c>
@@ -68476,7 +68482,7 @@
       <c r="R89" s="494"/>
       <c r="W89" s="381"/>
     </row>
-    <row r="90" spans="1:24" s="111" customFormat="1" ht="12.95" customHeight="1">
+    <row r="90" spans="1:24" s="111" customFormat="1" ht="13" customHeight="1">
       <c r="A90" s="112">
         <v>2016</v>
       </c>
@@ -68527,7 +68533,7 @@
       <c r="R90" s="494"/>
       <c r="W90" s="381"/>
     </row>
-    <row r="91" spans="1:24" s="111" customFormat="1" ht="12.95" customHeight="1">
+    <row r="91" spans="1:24" s="111" customFormat="1" ht="13" customHeight="1">
       <c r="A91" s="112">
         <v>2017</v>
       </c>
@@ -68578,7 +68584,7 @@
       <c r="R91" s="494"/>
       <c r="W91" s="381"/>
     </row>
-    <row r="92" spans="1:24" s="111" customFormat="1" ht="12.95" customHeight="1">
+    <row r="92" spans="1:24" s="111" customFormat="1" ht="13" customHeight="1">
       <c r="A92" s="153">
         <v>2018</v>
       </c>
@@ -68654,7 +68660,7 @@
       <c r="V93" s="381"/>
       <c r="W93" s="381"/>
     </row>
-    <row r="94" spans="1:24" s="111" customFormat="1" ht="12.95" customHeight="1">
+    <row r="94" spans="1:24" s="111" customFormat="1" ht="13" customHeight="1">
       <c r="A94" s="159" t="s">
         <v>145</v>
       </c>
@@ -68679,7 +68685,7 @@
       <c r="V94" s="381"/>
       <c r="W94" s="381"/>
     </row>
-    <row r="95" spans="1:24" s="111" customFormat="1" ht="12.95" customHeight="1">
+    <row r="95" spans="1:24" s="111" customFormat="1" ht="13" customHeight="1">
       <c r="A95" s="159" t="s">
         <v>435</v>
       </c>
@@ -68698,7 +68704,7 @@
       <c r="N95" s="114"/>
       <c r="O95" s="114"/>
     </row>
-    <row r="96" spans="1:24" s="111" customFormat="1" ht="10.35" customHeight="1">
+    <row r="96" spans="1:24" s="111" customFormat="1" ht="10.4" customHeight="1">
       <c r="A96" s="57" t="s">
         <v>146</v>
       </c>

</xml_diff>